<commit_message>
Add a test null i/o multiplexer, useful for optimising the i/o multiplexer implementation.
</commit_message>
<xml_diff>
--- a/programs/benchmark-async/results.xlsx
+++ b/programs/benchmark-async/results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="90" windowWidth="20505" windowHeight="10905"/>
+    <workbookView xWindow="-105" yWindow="90" windowWidth="29625" windowHeight="14295"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="20">
   <si>
     <t>LLFIO pipe_handle, no locking</t>
   </si>
@@ -67,6 +67,15 @@
   </si>
   <si>
     <t>ASIO over LLFIO</t>
+  </si>
+  <si>
+    <t>null multiplexer, no locking</t>
+  </si>
+  <si>
+    <t>null multiplexer, locking</t>
+  </si>
+  <si>
+    <t>locking over no locking</t>
   </si>
 </sst>
 </file>
@@ -160,7 +169,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$60</c:f>
+              <c:f>Sheet1!$H$77</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -195,21 +204,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$60:$E$60</c:f>
+              <c:f>Sheet1!$I$77:$L$77</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.29927000693795064</c:v>
+                  <c:v>0.14109586550623454</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.31286965333292899</c:v>
+                  <c:v>0.34469735216933217</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.3485234965172177</c:v>
+                  <c:v>0.37141506174186617</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.34342979884473601</c:v>
+                  <c:v>0.30987925625776092</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -220,7 +229,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$61</c:f>
+              <c:f>Sheet1!$H$78</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -255,21 +264,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$61:$E$61</c:f>
+              <c:f>Sheet1!$I$78:$L$78</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.63371504241312493</c:v>
+                  <c:v>-3.3015461894670792E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.17128534624577085</c:v>
+                  <c:v>0.43197638718587822</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.54447441991349932</c:v>
+                  <c:v>0.39895505745514753</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.37965381888833455</c:v>
+                  <c:v>0.22757844942487124</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -280,7 +289,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$62</c:f>
+              <c:f>Sheet1!$H$79</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -315,21 +324,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$62:$E$62</c:f>
+              <c:f>Sheet1!$I$79:$L$79</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.26666666666666666</c:v>
+                  <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.31164383561643838</c:v>
+                  <c:v>0.31661442006269591</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.32964824120603015</c:v>
+                  <c:v>0.36565403036079513</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.32653157093674123</c:v>
+                  <c:v>0.33716728228171045</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -340,7 +349,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$63</c:f>
+              <c:f>Sheet1!$H$80</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -375,32 +384,32 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$63:$E$63</c:f>
+              <c:f>Sheet1!$I$80:$L$80</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.54098360655737709</c:v>
+                  <c:v>0.13513513513513514</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.31753554502369669</c:v>
+                  <c:v>0.25840978593272174</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.38305585823500721</c:v>
+                  <c:v>0.29140753355289317</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.39044444754347551</c:v>
+                  <c:v>0.2449893690988422</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="167018880"/>
-        <c:axId val="167021568"/>
+        <c:axId val="154088576"/>
+        <c:axId val="154090880"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="167018880"/>
+        <c:axId val="154088576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -430,14 +439,14 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="167021568"/>
+        <c:crossAx val="154090880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="167021568"/>
+        <c:axId val="154090880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -469,7 +478,7 @@
         </c:title>
         <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="167018880"/>
+        <c:crossAx val="154088576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -482,7 +491,371 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>I/O</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> latencies null multiplexer</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$H$26</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Means</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$54:$E$54</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>64</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$I$26:$L$26</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.29754874498314704</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.17981585220821283</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.22963049901258883</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.24316471991590982</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$H$27</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Stddevs</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$54:$E$54</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>64</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$I$27:$L$27</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>-5.7982551054293133E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-172.1621603376868</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.4294342031561524E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.3574085988419247E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$H$28</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>50%s</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$54:$E$54</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>64</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$I$28:$L$28</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2638888888888889</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.25187533462138317</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$H$29</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>95%s</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$54:$E$54</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>64</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$I$29:$L$29</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.33333333333333331</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.13793103448275862</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.21967963386727687</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.22354530127888667</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="169813504"/>
+        <c:axId val="169815424"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="169813504"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Handles</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> in i/o multiplexer doing i/o</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="169815424"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="169815424"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Percentage</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> no locking is faster than locking</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="169813504"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -492,16 +865,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>514350</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>542925</xdr:colOff>
-      <xdr:row>65</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -515,6 +888,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -808,10 +1211,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E66"/>
+  <dimension ref="A1:L83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="C63" sqref="C63"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -823,7 +1226,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -848,16 +1251,16 @@
         <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>5.3499999999999999E-5</v>
+        <v>6.9999999999999999E-6</v>
       </c>
       <c r="C4" s="1">
-        <v>3.4150000000000003E-5</v>
+        <v>2.7999999999999999E-6</v>
       </c>
       <c r="D4" s="1">
-        <v>1.3556200000000001E-5</v>
+        <v>1.6937500000000001E-6</v>
       </c>
       <c r="E4" s="1">
-        <v>1.11453E-5</v>
+        <v>7.1093800000000004E-7</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -867,11 +1270,11 @@
       <c r="B5">
         <v>0</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
+        <v>2.4999999999999999E-8</v>
+      </c>
+      <c r="D5">
         <v>0</v>
-      </c>
-      <c r="D5" s="1">
-        <v>6.2499999999999997E-9</v>
       </c>
       <c r="E5" s="1">
         <v>1.5624999999999999E-9</v>
@@ -882,16 +1285,16 @@
         <v>4</v>
       </c>
       <c r="B6" s="1">
-        <v>1.8199999999999999E-5</v>
+        <v>6.0000000000000002E-6</v>
       </c>
       <c r="C6" s="1">
-        <v>7.0249999999999997E-6</v>
+        <v>9.5000000000000001E-7</v>
       </c>
       <c r="D6" s="1">
-        <v>4.6750000000000001E-6</v>
+        <v>7.1249999999999995E-7</v>
       </c>
       <c r="E6" s="1">
-        <v>3.25625E-6</v>
+        <v>1.8437500000000001E-7</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -899,33 +1302,33 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>1800</v>
+        <v>100</v>
       </c>
       <c r="C7">
-        <v>3500</v>
+        <v>300</v>
       </c>
       <c r="D7">
-        <v>10100</v>
+        <v>1200</v>
       </c>
       <c r="E7">
-        <v>35500</v>
+        <v>4700</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B8">
-        <v>344200</v>
-      </c>
-      <c r="C8">
-        <v>321200</v>
+      <c r="B8" s="1">
+        <v>349408000</v>
+      </c>
+      <c r="C8" s="1">
+        <v>447648000</v>
       </c>
       <c r="D8">
-        <v>494200</v>
+        <v>387200</v>
       </c>
       <c r="E8">
-        <v>550900</v>
+        <v>379100</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -933,16 +1336,16 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>2484.6999999999998</v>
+        <v>152.97</v>
       </c>
       <c r="C9">
-        <v>5770.29</v>
+        <v>457.24200000000002</v>
       </c>
       <c r="D9">
-        <v>17392.2</v>
+        <v>1509.67</v>
       </c>
       <c r="E9">
-        <v>68961.399999999994</v>
+        <v>5767.38</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -950,16 +1353,16 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>1126.92</v>
+        <v>66587.199999999997</v>
       </c>
       <c r="C10">
-        <v>2508.58</v>
+        <v>87215.2</v>
       </c>
       <c r="D10">
-        <v>6125.96</v>
+        <v>944.99699999999996</v>
       </c>
       <c r="E10">
-        <v>26275.599999999999</v>
+        <v>3311.88</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -967,16 +1370,16 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>2200</v>
+        <v>100</v>
       </c>
       <c r="C11">
-        <v>4900</v>
+        <v>400</v>
       </c>
       <c r="D11">
-        <v>15675</v>
+        <v>1325</v>
       </c>
       <c r="E11">
-        <v>61817.2</v>
+        <v>5142.1899999999996</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -984,16 +1387,16 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>3800</v>
+        <v>200</v>
       </c>
       <c r="C12">
-        <v>12100</v>
+        <v>625</v>
       </c>
       <c r="D12">
-        <v>26325</v>
+        <v>2131.25</v>
       </c>
       <c r="E12">
-        <v>135423</v>
+        <v>8335.94</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -1001,16 +1404,16 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>6700</v>
+        <v>300</v>
       </c>
       <c r="C13">
-        <v>13725</v>
+        <v>950</v>
       </c>
       <c r="D13">
-        <v>38337.5</v>
+        <v>3287.5</v>
       </c>
       <c r="E13">
-        <v>152256</v>
+        <v>12454.7</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -1018,16 +1421,16 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>8700</v>
+        <v>1500</v>
       </c>
       <c r="C14">
-        <v>18650</v>
+        <v>3800</v>
       </c>
       <c r="D14">
-        <v>51443.8</v>
+        <v>11725</v>
       </c>
       <c r="E14">
-        <v>203555</v>
+        <v>45756.3</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -1035,24 +1438,27 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>32100</v>
+        <v>3800</v>
       </c>
       <c r="C15">
-        <v>42800</v>
+        <v>9250</v>
       </c>
       <c r="D15">
-        <v>78737.5</v>
+        <v>27293.8</v>
       </c>
       <c r="E15">
-        <v>282969</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
+        <v>79676.600000000006</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
       <c r="A18" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
+        <v>18</v>
+      </c>
+      <c r="H18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
       <c r="A20" t="s">
         <v>1</v>
       </c>
@@ -1068,25 +1474,59 @@
       <c r="E20">
         <v>64</v>
       </c>
-    </row>
-    <row r="21" spans="1:5">
+      <c r="H20" t="s">
+        <v>1</v>
+      </c>
+      <c r="I20">
+        <v>1</v>
+      </c>
+      <c r="J20">
+        <v>4</v>
+      </c>
+      <c r="K20">
+        <v>16</v>
+      </c>
+      <c r="L20">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
       <c r="A21" t="s">
         <v>2</v>
       </c>
       <c r="B21" s="1">
-        <v>7.4900000000000005E-5</v>
+        <v>1.5400000000000002E-5</v>
       </c>
       <c r="C21" s="1">
-        <v>2.5199999999999999E-5</v>
+        <v>3.4750000000000002E-6</v>
       </c>
       <c r="D21" s="1">
-        <v>1.4175000000000001E-5</v>
+        <v>1.8125E-6</v>
       </c>
       <c r="E21" s="1">
-        <v>9.1531299999999992E-6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
+        <v>7.1249999999999995E-7</v>
+      </c>
+      <c r="H21" t="s">
+        <v>2</v>
+      </c>
+      <c r="I21" s="2">
+        <f>(B21-B4)/B21</f>
+        <v>0.54545454545454541</v>
+      </c>
+      <c r="J21" s="2">
+        <f>(C21-C4)/C21</f>
+        <v>0.19424460431654683</v>
+      </c>
+      <c r="K21" s="2">
+        <f>(D21-D4)/D21</f>
+        <v>6.5517241379310295E-2</v>
+      </c>
+      <c r="L21" s="2">
+        <f>(E21-E4)/E21</f>
+        <v>2.1922807017542715E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
       <c r="A22" t="s">
         <v>3</v>
       </c>
@@ -1096,186 +1536,395 @@
       <c r="C22" s="1">
         <v>2.4999999999999999E-8</v>
       </c>
-      <c r="D22" s="1">
-        <v>6.2499999999999997E-9</v>
+      <c r="D22">
+        <v>0</v>
       </c>
       <c r="E22" s="1">
         <v>1.5624999999999999E-9</v>
       </c>
-    </row>
-    <row r="23" spans="1:5">
+      <c r="H22" t="s">
+        <v>3</v>
+      </c>
+      <c r="I22" s="2">
+        <f>(B22-B5)/B22</f>
+        <v>1</v>
+      </c>
+      <c r="J22" s="2">
+        <f>(C22-C5)/C22</f>
+        <v>0</v>
+      </c>
+      <c r="K22" s="2" t="e">
+        <f>(D22-D5)/D22</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L22" s="2">
+        <f>(E22-E5)/E22</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
       <c r="A23" t="s">
         <v>4</v>
       </c>
       <c r="B23" s="1">
-        <v>1.77E-5</v>
+        <v>4.1999999999999996E-6</v>
       </c>
       <c r="C23" s="1">
-        <v>7.525E-6</v>
+        <v>1.15E-6</v>
       </c>
       <c r="D23" s="1">
-        <v>4.1125E-6</v>
+        <v>2.6875000000000002E-7</v>
       </c>
       <c r="E23" s="1">
-        <v>4.4078100000000002E-6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
+        <v>1.42187E-7</v>
+      </c>
+      <c r="H23" t="s">
+        <v>4</v>
+      </c>
+      <c r="I23" s="2">
+        <f>(B23-B6)/B23</f>
+        <v>-0.42857142857142877</v>
+      </c>
+      <c r="J23" s="2">
+        <f>(C23-C6)/C23</f>
+        <v>0.17391304347826086</v>
+      </c>
+      <c r="K23" s="2">
+        <f>(D23-D6)/D23</f>
+        <v>-1.651162790697674</v>
+      </c>
+      <c r="L23" s="2">
+        <f>(E23-E6)/E23</f>
+        <v>-0.29670785655510001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
       <c r="A24" t="s">
         <v>5</v>
       </c>
       <c r="B24">
-        <v>2000</v>
+        <v>100</v>
       </c>
       <c r="C24">
-        <v>3900</v>
+        <v>400</v>
       </c>
       <c r="D24">
-        <v>11200</v>
+        <v>1600</v>
       </c>
       <c r="E24">
-        <v>39700</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
+        <v>6400</v>
+      </c>
+      <c r="H24" t="s">
+        <v>5</v>
+      </c>
+      <c r="I24" s="2">
+        <f>(B24-B7)/B24</f>
+        <v>0</v>
+      </c>
+      <c r="J24" s="2">
+        <f>(C24-C7)/C24</f>
+        <v>0.25</v>
+      </c>
+      <c r="K24" s="2">
+        <f>(D24-D7)/D24</f>
+        <v>0.25</v>
+      </c>
+      <c r="L24" s="2">
+        <f>(E24-E7)/E24</f>
+        <v>0.265625</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
       <c r="A25" t="s">
         <v>6</v>
       </c>
-      <c r="B25">
-        <v>325100</v>
+      <c r="B25" s="1">
+        <v>266671000</v>
       </c>
       <c r="C25" s="1">
-        <v>2028500</v>
+        <v>1736700</v>
       </c>
       <c r="D25">
-        <v>196800</v>
+        <v>258800</v>
       </c>
       <c r="E25">
-        <v>513000</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
+        <v>680900</v>
+      </c>
+      <c r="H25" t="s">
+        <v>6</v>
+      </c>
+      <c r="I25" s="2">
+        <f>(B25-B8)/B25</f>
+        <v>-0.31025870829599017</v>
+      </c>
+      <c r="J25" s="2">
+        <f>(C25-C8)/C25</f>
+        <v>-256.75781654862669</v>
+      </c>
+      <c r="K25" s="2">
+        <f>(D25-D8)/D25</f>
+        <v>-0.49613601236476046</v>
+      </c>
+      <c r="L25" s="2">
+        <f>(E25-E8)/E25</f>
+        <v>0.44323689234836244</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
       <c r="A26" t="s">
         <v>7</v>
       </c>
       <c r="B26">
-        <v>2322.9899999999998</v>
+        <v>217.76599999999999</v>
       </c>
       <c r="C26">
-        <v>5438.3</v>
+        <v>557.48699999999997</v>
       </c>
       <c r="D26">
-        <v>17265.3</v>
+        <v>1959.67</v>
       </c>
       <c r="E26">
-        <v>67858.5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
+        <v>7620.39</v>
+      </c>
+      <c r="H26" t="s">
+        <v>7</v>
+      </c>
+      <c r="I26" s="2">
+        <f>(B26-B9)/B26</f>
+        <v>0.29754874498314704</v>
+      </c>
+      <c r="J26" s="2">
+        <f>(C26-C9)/C26</f>
+        <v>0.17981585220821283</v>
+      </c>
+      <c r="K26" s="2">
+        <f>(D26-D9)/D26</f>
+        <v>0.22963049901258883</v>
+      </c>
+      <c r="L26" s="2">
+        <f>(E26-E9)/E26</f>
+        <v>0.24316471991590982</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
       <c r="A27" t="s">
         <v>8</v>
       </c>
       <c r="B27">
-        <v>674.91300000000001</v>
+        <v>62937.9</v>
       </c>
       <c r="C27">
-        <v>2669.87</v>
+        <v>503.66199999999998</v>
       </c>
       <c r="D27">
-        <v>3723.17</v>
+        <v>958.70100000000002</v>
       </c>
       <c r="E27">
-        <v>18901.7</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
+        <v>3574.9</v>
+      </c>
+      <c r="H27" t="s">
+        <v>8</v>
+      </c>
+      <c r="I27" s="2">
+        <f>(B27-B10)/B27</f>
+        <v>-5.7982551054293133E-2</v>
+      </c>
+      <c r="J27" s="2">
+        <f>(C27-C10)/C27</f>
+        <v>-172.1621603376868</v>
+      </c>
+      <c r="K27" s="2">
+        <f>(D27-D10)/D27</f>
+        <v>1.4294342031561524E-2</v>
+      </c>
+      <c r="L27" s="2">
+        <f>(E27-E10)/E27</f>
+        <v>7.3574085988419247E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
       <c r="A28" t="s">
         <v>9</v>
       </c>
       <c r="B28">
-        <v>2200</v>
+        <v>200</v>
       </c>
       <c r="C28">
-        <v>5025</v>
+        <v>500</v>
       </c>
       <c r="D28">
-        <v>16675</v>
+        <v>1800</v>
       </c>
       <c r="E28">
-        <v>64514.1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
+        <v>6873.44</v>
+      </c>
+      <c r="H28" t="s">
+        <v>9</v>
+      </c>
+      <c r="I28" s="2">
+        <f>(B28-B11)/B28</f>
+        <v>0.5</v>
+      </c>
+      <c r="J28" s="2">
+        <f>(C28-C11)/C28</f>
+        <v>0.2</v>
+      </c>
+      <c r="K28" s="2">
+        <f>(D28-D11)/D28</f>
+        <v>0.2638888888888889</v>
+      </c>
+      <c r="L28" s="2">
+        <f>(E28-E11)/E28</f>
+        <v>0.25187533462138317</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
       <c r="A29" t="s">
         <v>10</v>
       </c>
       <c r="B29">
-        <v>2800</v>
+        <v>300</v>
       </c>
       <c r="C29">
-        <v>7200</v>
+        <v>725</v>
       </c>
       <c r="D29">
-        <v>21118.799999999999</v>
+        <v>2731.25</v>
       </c>
       <c r="E29">
-        <v>87418.8</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
+        <v>10735.9</v>
+      </c>
+      <c r="H29" t="s">
+        <v>10</v>
+      </c>
+      <c r="I29" s="2">
+        <f>(B29-B12)/B29</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="J29" s="2">
+        <f>(C29-C12)/C29</f>
+        <v>0.13793103448275862</v>
+      </c>
+      <c r="K29" s="2">
+        <f>(D29-D12)/D29</f>
+        <v>0.21967963386727687</v>
+      </c>
+      <c r="L29" s="2">
+        <f>(E29-E12)/E29</f>
+        <v>0.22354530127888667</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12">
       <c r="A30" t="s">
         <v>11</v>
       </c>
       <c r="B30">
-        <v>5500</v>
+        <v>400</v>
       </c>
       <c r="C30">
-        <v>12525</v>
+        <v>1100</v>
       </c>
       <c r="D30">
-        <v>26143.8</v>
+        <v>4150</v>
       </c>
       <c r="E30">
-        <v>147325</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
+        <v>16279.7</v>
+      </c>
+      <c r="H30" t="s">
+        <v>11</v>
+      </c>
+      <c r="I30" s="2">
+        <f>(B30-B13)/B30</f>
+        <v>0.25</v>
+      </c>
+      <c r="J30" s="2">
+        <f>(C30-C13)/C30</f>
+        <v>0.13636363636363635</v>
+      </c>
+      <c r="K30" s="2">
+        <f>(D30-D13)/D30</f>
+        <v>0.20783132530120482</v>
+      </c>
+      <c r="L30" s="2">
+        <f>(E30-E13)/E30</f>
+        <v>0.23495518959194578</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12">
       <c r="A31" t="s">
         <v>12</v>
       </c>
       <c r="B31">
-        <v>7500</v>
+        <v>1600</v>
       </c>
       <c r="C31">
-        <v>16775</v>
+        <v>3825</v>
       </c>
       <c r="D31">
-        <v>38668.800000000003</v>
+        <v>12643.8</v>
       </c>
       <c r="E31">
-        <v>192634</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
+        <v>49046.9</v>
+      </c>
+      <c r="H31" t="s">
+        <v>12</v>
+      </c>
+      <c r="I31" s="2">
+        <f>(B31-B14)/B31</f>
+        <v>6.25E-2</v>
+      </c>
+      <c r="J31" s="2">
+        <f>(C31-C14)/C31</f>
+        <v>6.5359477124183009E-3</v>
+      </c>
+      <c r="K31" s="2">
+        <f>(D31-D14)/D31</f>
+        <v>7.2668027017194145E-2</v>
+      </c>
+      <c r="L31" s="2">
+        <f>(E31-E14)/E31</f>
+        <v>6.7090886478044454E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12">
       <c r="A32" t="s">
         <v>13</v>
       </c>
       <c r="B32">
-        <v>22500</v>
+        <v>4100</v>
       </c>
       <c r="C32">
-        <v>38750</v>
+        <v>9950</v>
       </c>
       <c r="D32">
-        <v>61212.5</v>
+        <v>28087.5</v>
       </c>
       <c r="E32">
-        <v>247348</v>
+        <v>86120.3</v>
+      </c>
+      <c r="H32" t="s">
+        <v>13</v>
+      </c>
+      <c r="I32" s="2">
+        <f>(B32-B15)/B32</f>
+        <v>7.3170731707317069E-2</v>
+      </c>
+      <c r="J32" s="2">
+        <f>(C32-C15)/C32</f>
+        <v>7.0351758793969849E-2</v>
+      </c>
+      <c r="K32" s="2">
+        <f>(D32-D15)/D32</f>
+        <v>2.8258121940364957E-2</v>
+      </c>
+      <c r="L32" s="2">
+        <f>(E32-E15)/E32</f>
+        <v>7.4822080276078895E-2</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" t="s">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -1300,16 +1949,16 @@
         <v>2</v>
       </c>
       <c r="B38" s="1">
-        <v>6.9900000000000005E-5</v>
+        <v>8.4800000000000001E-5</v>
       </c>
       <c r="C38" s="1">
-        <v>2.8099999999999999E-5</v>
+        <v>2.6825000000000002E-5</v>
       </c>
       <c r="D38" s="1">
-        <v>1.9037499999999999E-5</v>
+        <v>1.4E-5</v>
       </c>
       <c r="E38" s="1">
-        <v>1.1535900000000001E-5</v>
+        <v>1.20625E-5</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -1317,33 +1966,33 @@
         <v>3</v>
       </c>
       <c r="B39">
-        <v>3.7979599999999998</v>
+        <v>0</v>
       </c>
       <c r="C39">
-        <v>1.37405</v>
-      </c>
-      <c r="D39">
-        <v>0.383017</v>
-      </c>
-      <c r="E39">
-        <v>9.7711400000000004E-2</v>
+        <v>0</v>
+      </c>
+      <c r="D39" s="1">
+        <v>6.2499999999999997E-9</v>
+      </c>
+      <c r="E39" s="1">
+        <v>1.5624999999999999E-9</v>
       </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" t="s">
         <v>4</v>
       </c>
-      <c r="B40">
-        <v>2.1401500000000002</v>
-      </c>
-      <c r="C40">
-        <v>0.803539</v>
-      </c>
-      <c r="D40">
-        <v>0.236401</v>
-      </c>
-      <c r="E40">
-        <v>6.3788600000000001E-2</v>
+      <c r="B40" s="1">
+        <v>2.2900000000000001E-5</v>
+      </c>
+      <c r="C40" s="1">
+        <v>8.1499999999999999E-6</v>
+      </c>
+      <c r="D40" s="1">
+        <v>4.5125000000000004E-6</v>
+      </c>
+      <c r="E40" s="1">
+        <v>3.55938E-6</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -1351,33 +2000,33 @@
         <v>5</v>
       </c>
       <c r="B41">
-        <v>2500</v>
+        <v>1800</v>
       </c>
       <c r="C41">
-        <v>4800</v>
+        <v>3500</v>
       </c>
       <c r="D41">
-        <v>14100</v>
+        <v>10100</v>
       </c>
       <c r="E41">
-        <v>52600</v>
+        <v>35200</v>
       </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" t="s">
         <v>6</v>
       </c>
-      <c r="B42">
-        <v>195300</v>
+      <c r="B42" s="1">
+        <v>1735200</v>
       </c>
       <c r="C42">
-        <v>279900</v>
+        <v>597300</v>
       </c>
       <c r="D42">
-        <v>383600</v>
+        <v>296900</v>
       </c>
       <c r="E42">
-        <v>664000</v>
+        <v>718000</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -1385,16 +2034,16 @@
         <v>7</v>
       </c>
       <c r="B43">
-        <v>3315.1</v>
+        <v>2797.39</v>
       </c>
       <c r="C43">
-        <v>7914.51</v>
+        <v>6067.99</v>
       </c>
       <c r="D43">
-        <v>26501.8</v>
+        <v>20019.7</v>
       </c>
       <c r="E43">
-        <v>103353</v>
+        <v>82234.8</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -1402,16 +2051,16 @@
         <v>8</v>
       </c>
       <c r="B44">
-        <v>1842.59</v>
+        <v>1916.54</v>
       </c>
       <c r="C44">
-        <v>3221.7</v>
+        <v>2926.52</v>
       </c>
       <c r="D44">
-        <v>8173.35</v>
+        <v>8824.73</v>
       </c>
       <c r="E44">
-        <v>30469.599999999999</v>
+        <v>37723.599999999999</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -1419,16 +2068,16 @@
         <v>9</v>
       </c>
       <c r="B45">
-        <v>3000</v>
+        <v>2200</v>
       </c>
       <c r="C45">
-        <v>7300</v>
+        <v>5175</v>
       </c>
       <c r="D45">
-        <v>24875</v>
+        <v>16875</v>
       </c>
       <c r="E45">
-        <v>95793.8</v>
+        <v>67831.3</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -1436,16 +2085,16 @@
         <v>10</v>
       </c>
       <c r="B46">
-        <v>6100</v>
+        <v>6000</v>
       </c>
       <c r="C46">
-        <v>10550</v>
+        <v>11650</v>
       </c>
       <c r="D46">
-        <v>34231.300000000003</v>
+        <v>37200</v>
       </c>
       <c r="E46">
-        <v>143414</v>
+        <v>144358</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -1453,16 +2102,16 @@
         <v>11</v>
       </c>
       <c r="B47">
-        <v>7700</v>
+        <v>7000</v>
       </c>
       <c r="C47">
-        <v>16375</v>
+        <v>14150</v>
       </c>
       <c r="D47">
-        <v>57575</v>
+        <v>44187.5</v>
       </c>
       <c r="E47">
-        <v>195903</v>
+        <v>175428</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -1470,16 +2119,16 @@
         <v>12</v>
       </c>
       <c r="B48">
-        <v>36200</v>
+        <v>10900</v>
       </c>
       <c r="C48">
-        <v>48000</v>
+        <v>23175</v>
       </c>
       <c r="D48">
-        <v>85012.5</v>
+        <v>62856.3</v>
       </c>
       <c r="E48">
-        <v>248303</v>
+        <v>237444</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -1487,21 +2136,21 @@
         <v>13</v>
       </c>
       <c r="B49">
-        <v>61100</v>
+        <v>36300</v>
       </c>
       <c r="C49">
-        <v>76675</v>
+        <v>60025</v>
       </c>
       <c r="D49">
-        <v>115744</v>
+        <v>116219</v>
       </c>
       <c r="E49">
-        <v>343616</v>
+        <v>340753</v>
       </c>
     </row>
     <row r="52" spans="1:5">
       <c r="A52" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -1525,252 +2174,676 @@
       <c r="A55" t="s">
         <v>2</v>
       </c>
-      <c r="B55" s="2">
-        <f>(B38-B21)/B38</f>
-        <v>-7.1530758226037189E-2</v>
-      </c>
-      <c r="C55" s="2">
-        <f t="shared" ref="C55:E55" si="0">(C38-C21)/C38</f>
-        <v>0.10320284697508895</v>
-      </c>
-      <c r="D55" s="2">
-        <f t="shared" si="0"/>
-        <v>0.25541694024950745</v>
-      </c>
-      <c r="E55" s="2">
-        <f t="shared" si="0"/>
-        <v>0.20655258800787121</v>
+      <c r="B55" s="1">
+        <v>4.4499999999999997E-5</v>
+      </c>
+      <c r="C55" s="1">
+        <v>2.3275E-5</v>
+      </c>
+      <c r="D55" s="1">
+        <v>1.3468800000000001E-5</v>
+      </c>
+      <c r="E55" s="1">
+        <v>1.05984E-5</v>
       </c>
     </row>
     <row r="56" spans="1:5">
       <c r="A56" t="s">
         <v>3</v>
       </c>
-      <c r="B56" s="2">
-        <f t="shared" ref="B56:E66" si="1">(B39-B22)/B39</f>
-        <v>0.99999997367007554</v>
-      </c>
-      <c r="C56" s="2">
-        <f t="shared" si="1"/>
-        <v>0.99999998180561112</v>
-      </c>
-      <c r="D56" s="2">
-        <f t="shared" si="1"/>
-        <v>0.99999998368218634</v>
-      </c>
-      <c r="E56" s="2">
-        <f t="shared" si="1"/>
-        <v>0.99999998400903067</v>
+      <c r="B56">
+        <v>0</v>
+      </c>
+      <c r="C56" s="1">
+        <v>2.4999999999999999E-8</v>
+      </c>
+      <c r="D56">
+        <v>0</v>
+      </c>
+      <c r="E56" s="1">
+        <v>1.5624999999999999E-9</v>
       </c>
     </row>
     <row r="57" spans="1:5">
       <c r="A57" t="s">
         <v>4</v>
       </c>
-      <c r="B57" s="2">
-        <f t="shared" si="1"/>
-        <v>0.99999172955166704</v>
-      </c>
-      <c r="C57" s="2">
-        <f t="shared" si="1"/>
-        <v>0.99999063517763298</v>
-      </c>
-      <c r="D57" s="2">
-        <f t="shared" si="1"/>
-        <v>0.99998260371149028</v>
-      </c>
-      <c r="E57" s="2">
-        <f t="shared" si="1"/>
-        <v>0.99993089972189397</v>
+      <c r="B57" s="1">
+        <v>2.5299999999999998E-5</v>
+      </c>
+      <c r="C57" s="1">
+        <v>9.3500000000000003E-6</v>
+      </c>
+      <c r="D57" s="1">
+        <v>5.0499999999999999E-6</v>
+      </c>
+      <c r="E57" s="1">
+        <v>3.80313E-6</v>
       </c>
     </row>
     <row r="58" spans="1:5">
       <c r="A58" t="s">
         <v>5</v>
       </c>
-      <c r="B58" s="2">
-        <f t="shared" si="1"/>
-        <v>0.2</v>
-      </c>
-      <c r="C58" s="2">
-        <f t="shared" si="1"/>
-        <v>0.1875</v>
-      </c>
-      <c r="D58" s="2">
-        <f t="shared" si="1"/>
-        <v>0.20567375886524822</v>
-      </c>
-      <c r="E58" s="2">
-        <f t="shared" si="1"/>
-        <v>0.24524714828897337</v>
+      <c r="B58">
+        <v>1900</v>
+      </c>
+      <c r="C58">
+        <v>3800</v>
+      </c>
+      <c r="D58">
+        <v>10900</v>
+      </c>
+      <c r="E58">
+        <v>38900</v>
       </c>
     </row>
     <row r="59" spans="1:5">
       <c r="A59" t="s">
         <v>6</v>
       </c>
-      <c r="B59" s="2">
-        <f t="shared" si="1"/>
-        <v>-0.66461853558627748</v>
-      </c>
-      <c r="C59" s="2">
-        <f t="shared" si="1"/>
-        <v>-6.2472311539835657</v>
-      </c>
-      <c r="D59" s="2">
-        <f t="shared" si="1"/>
-        <v>0.48696558915537019</v>
-      </c>
-      <c r="E59" s="2">
-        <f t="shared" si="1"/>
-        <v>0.22740963855421686</v>
+      <c r="B59" s="1">
+        <v>2051500</v>
+      </c>
+      <c r="C59">
+        <v>535800</v>
+      </c>
+      <c r="D59">
+        <v>493400</v>
+      </c>
+      <c r="E59" s="1">
+        <v>3511800</v>
       </c>
     </row>
     <row r="60" spans="1:5">
       <c r="A60" t="s">
         <v>7</v>
       </c>
-      <c r="B60" s="2">
-        <f t="shared" si="1"/>
-        <v>0.29927000693795064</v>
-      </c>
-      <c r="C60" s="2">
-        <f t="shared" si="1"/>
-        <v>0.31286965333292899</v>
-      </c>
-      <c r="D60" s="2">
-        <f t="shared" si="1"/>
-        <v>0.3485234965172177</v>
-      </c>
-      <c r="E60" s="2">
-        <f t="shared" si="1"/>
-        <v>0.34342979884473601</v>
+      <c r="B60">
+        <v>3307.03</v>
+      </c>
+      <c r="C60">
+        <v>6425</v>
+      </c>
+      <c r="D60">
+        <v>20738.400000000001</v>
+      </c>
+      <c r="E60">
+        <v>84476.3</v>
       </c>
     </row>
     <row r="61" spans="1:5">
       <c r="A61" t="s">
         <v>8</v>
       </c>
-      <c r="B61" s="2">
-        <f t="shared" si="1"/>
-        <v>0.63371504241312493</v>
-      </c>
-      <c r="C61" s="2">
-        <f t="shared" si="1"/>
-        <v>0.17128534624577085</v>
-      </c>
-      <c r="D61" s="2">
-        <f t="shared" si="1"/>
-        <v>0.54447441991349932</v>
-      </c>
-      <c r="E61" s="2">
-        <f t="shared" si="1"/>
-        <v>0.37965381888833455</v>
+      <c r="B61">
+        <v>2632.33</v>
+      </c>
+      <c r="C61">
+        <v>2969.44</v>
+      </c>
+      <c r="D61">
+        <v>9001.7900000000009</v>
+      </c>
+      <c r="E61">
+        <v>40103.199999999997</v>
       </c>
     </row>
     <row r="62" spans="1:5">
       <c r="A62" t="s">
         <v>9</v>
       </c>
-      <c r="B62" s="2">
-        <f t="shared" si="1"/>
-        <v>0.26666666666666666</v>
-      </c>
-      <c r="C62" s="2">
-        <f t="shared" si="1"/>
-        <v>0.31164383561643838</v>
-      </c>
-      <c r="D62" s="2">
-        <f t="shared" si="1"/>
-        <v>0.32964824120603015</v>
-      </c>
-      <c r="E62" s="2">
-        <f t="shared" si="1"/>
-        <v>0.32653157093674123</v>
+      <c r="B62">
+        <v>2400</v>
+      </c>
+      <c r="C62">
+        <v>5450</v>
+      </c>
+      <c r="D62">
+        <v>17337.5</v>
+      </c>
+      <c r="E62">
+        <v>69626.600000000006</v>
       </c>
     </row>
     <row r="63" spans="1:5">
       <c r="A63" t="s">
         <v>10</v>
       </c>
-      <c r="B63" s="2">
-        <f t="shared" si="1"/>
-        <v>0.54098360655737709</v>
-      </c>
-      <c r="C63" s="2">
-        <f t="shared" si="1"/>
-        <v>0.31753554502369669</v>
-      </c>
-      <c r="D63" s="2">
-        <f t="shared" si="1"/>
-        <v>0.38305585823500721</v>
-      </c>
-      <c r="E63" s="2">
-        <f t="shared" si="1"/>
-        <v>0.39044444754347551</v>
+      <c r="B63">
+        <v>6400</v>
+      </c>
+      <c r="C63">
+        <v>12125</v>
+      </c>
+      <c r="D63">
+        <v>37781.300000000003</v>
+      </c>
+      <c r="E63">
+        <v>149853</v>
       </c>
     </row>
     <row r="64" spans="1:5">
       <c r="A64" t="s">
         <v>11</v>
       </c>
-      <c r="B64" s="2">
-        <f t="shared" si="1"/>
-        <v>0.2857142857142857</v>
-      </c>
-      <c r="C64" s="2">
-        <f t="shared" si="1"/>
-        <v>0.23511450381679388</v>
-      </c>
-      <c r="D64" s="2">
-        <f t="shared" si="1"/>
-        <v>0.5459174989144594</v>
-      </c>
-      <c r="E64" s="2">
-        <f t="shared" si="1"/>
-        <v>0.24796965845341828</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5">
+      <c r="B64">
+        <v>7500</v>
+      </c>
+      <c r="C64">
+        <v>14700</v>
+      </c>
+      <c r="D64">
+        <v>45787.5</v>
+      </c>
+      <c r="E64">
+        <v>179666</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12">
       <c r="A65" t="s">
         <v>12</v>
       </c>
-      <c r="B65" s="2">
-        <f t="shared" si="1"/>
-        <v>0.79281767955801108</v>
-      </c>
-      <c r="C65" s="2">
-        <f t="shared" si="1"/>
-        <v>0.65052083333333333</v>
-      </c>
-      <c r="D65" s="2">
-        <f t="shared" si="1"/>
-        <v>0.54513983237759145</v>
-      </c>
-      <c r="E65" s="2">
-        <f t="shared" si="1"/>
-        <v>0.22419785504001161</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5">
+      <c r="B65">
+        <v>12900</v>
+      </c>
+      <c r="C65">
+        <v>22900</v>
+      </c>
+      <c r="D65">
+        <v>64443.8</v>
+      </c>
+      <c r="E65">
+        <v>245831</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12">
       <c r="A66" t="s">
         <v>13</v>
       </c>
-      <c r="B66" s="2">
-        <f t="shared" si="1"/>
-        <v>0.6317512274959084</v>
-      </c>
-      <c r="C66" s="2">
-        <f t="shared" si="1"/>
-        <v>0.49462014998369741</v>
-      </c>
-      <c r="D66" s="2">
-        <f t="shared" si="1"/>
-        <v>0.47113889272878073</v>
-      </c>
-      <c r="E66" s="2">
-        <f t="shared" si="1"/>
-        <v>0.28016157571242317</v>
+      <c r="B66">
+        <v>41100</v>
+      </c>
+      <c r="C66">
+        <v>57325</v>
+      </c>
+      <c r="D66">
+        <v>111206</v>
+      </c>
+      <c r="E66">
+        <v>328900</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12">
+      <c r="A69" t="s">
+        <v>15</v>
+      </c>
+      <c r="H69" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12">
+      <c r="A71" t="s">
+        <v>1</v>
+      </c>
+      <c r="B71">
+        <v>1</v>
+      </c>
+      <c r="C71">
+        <v>4</v>
+      </c>
+      <c r="D71">
+        <v>16</v>
+      </c>
+      <c r="E71">
+        <v>64</v>
+      </c>
+      <c r="H71" t="s">
+        <v>1</v>
+      </c>
+      <c r="I71">
+        <v>1</v>
+      </c>
+      <c r="J71">
+        <v>4</v>
+      </c>
+      <c r="K71">
+        <v>16</v>
+      </c>
+      <c r="L71">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12">
+      <c r="A72" t="s">
+        <v>2</v>
+      </c>
+      <c r="B72" s="1">
+        <v>8.0599999999999994E-5</v>
+      </c>
+      <c r="C72" s="1">
+        <v>3.1000000000000001E-5</v>
+      </c>
+      <c r="D72" s="1">
+        <v>1.8575000000000001E-5</v>
+      </c>
+      <c r="E72" s="1">
+        <v>1.145E-5</v>
+      </c>
+      <c r="H72" t="s">
+        <v>2</v>
+      </c>
+      <c r="I72" s="2">
+        <f>(B72-B55)/B72</f>
+        <v>0.4478908188585608</v>
+      </c>
+      <c r="J72" s="2">
+        <f>(C72-C55)/C72</f>
+        <v>0.24919354838709681</v>
+      </c>
+      <c r="K72" s="2">
+        <f>(D72-D55)/D72</f>
+        <v>0.27489636608344548</v>
+      </c>
+      <c r="L72" s="2">
+        <f>(E72-E55)/E72</f>
+        <v>7.4375545851528418E-2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12">
+      <c r="A73" t="s">
+        <v>3</v>
+      </c>
+      <c r="B73">
+        <v>3.4744700000000002</v>
+      </c>
+      <c r="C73">
+        <v>1.18692</v>
+      </c>
+      <c r="D73">
+        <v>0.32213700000000001</v>
+      </c>
+      <c r="E73">
+        <v>9.1308399999999998E-2</v>
+      </c>
+      <c r="H73" t="s">
+        <v>3</v>
+      </c>
+      <c r="I73" s="2">
+        <f>(B73-B56)/B73</f>
+        <v>1</v>
+      </c>
+      <c r="J73" s="2">
+        <f>(C73-C56)/C73</f>
+        <v>0.99999997893708081</v>
+      </c>
+      <c r="K73" s="2">
+        <f>(D73-D56)/D73</f>
+        <v>1</v>
+      </c>
+      <c r="L73" s="2">
+        <f>(E73-E56)/E73</f>
+        <v>0.99999998288766423</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12">
+      <c r="A74" t="s">
+        <v>4</v>
+      </c>
+      <c r="B74">
+        <v>1.9770300000000001</v>
+      </c>
+      <c r="C74">
+        <v>0.66740500000000003</v>
+      </c>
+      <c r="D74">
+        <v>0.18677199999999999</v>
+      </c>
+      <c r="E74">
+        <v>5.2539000000000002E-2</v>
+      </c>
+      <c r="H74" t="s">
+        <v>4</v>
+      </c>
+      <c r="I74" s="2">
+        <f>(B74-B57)/B74</f>
+        <v>0.99998720302676247</v>
+      </c>
+      <c r="J74" s="2">
+        <f>(C74-C57)/C74</f>
+        <v>0.99998599051550408</v>
+      </c>
+      <c r="K74" s="2">
+        <f>(D74-D57)/D74</f>
+        <v>0.99997296168590577</v>
+      </c>
+      <c r="L74" s="2">
+        <f>(E74-E57)/E74</f>
+        <v>0.9999276132016216</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12">
+      <c r="A75" t="s">
+        <v>5</v>
+      </c>
+      <c r="B75">
+        <v>2500</v>
+      </c>
+      <c r="C75">
+        <v>4800</v>
+      </c>
+      <c r="D75">
+        <v>13900</v>
+      </c>
+      <c r="E75">
+        <v>51700</v>
+      </c>
+      <c r="H75" t="s">
+        <v>5</v>
+      </c>
+      <c r="I75" s="2">
+        <f>(B75-B58)/B75</f>
+        <v>0.24</v>
+      </c>
+      <c r="J75" s="2">
+        <f>(C75-C58)/C75</f>
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="K75" s="2">
+        <f>(D75-D58)/D75</f>
+        <v>0.21582733812949639</v>
+      </c>
+      <c r="L75" s="2">
+        <f>(E75-E58)/E75</f>
+        <v>0.24758220502901354</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12">
+      <c r="A76" t="s">
+        <v>6</v>
+      </c>
+      <c r="B76" s="1">
+        <v>1107800</v>
+      </c>
+      <c r="C76">
+        <v>683700</v>
+      </c>
+      <c r="D76" s="1">
+        <v>1897900</v>
+      </c>
+      <c r="E76" s="1">
+        <v>2647300</v>
+      </c>
+      <c r="H76" t="s">
+        <v>6</v>
+      </c>
+      <c r="I76" s="2">
+        <f>(B76-B59)/B76</f>
+        <v>-0.85186856833363422</v>
+      </c>
+      <c r="J76" s="2">
+        <f>(C76-C59)/C76</f>
+        <v>0.21632294866169371</v>
+      </c>
+      <c r="K76" s="2">
+        <f>(D76-D59)/D76</f>
+        <v>0.74002845250013172</v>
+      </c>
+      <c r="L76" s="2">
+        <f>(E76-E59)/E76</f>
+        <v>-0.32655913572318968</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12">
+      <c r="A77" t="s">
+        <v>7</v>
+      </c>
+      <c r="B77">
+        <v>3850.29</v>
+      </c>
+      <c r="C77">
+        <v>9804.6299999999992</v>
+      </c>
+      <c r="D77">
+        <v>32992.199999999997</v>
+      </c>
+      <c r="E77">
+        <v>122408</v>
+      </c>
+      <c r="H77" t="s">
+        <v>7</v>
+      </c>
+      <c r="I77" s="2">
+        <f>(B77-B60)/B77</f>
+        <v>0.14109586550623454</v>
+      </c>
+      <c r="J77" s="2">
+        <f>(C77-C60)/C77</f>
+        <v>0.34469735216933217</v>
+      </c>
+      <c r="K77" s="2">
+        <f>(D77-D60)/D77</f>
+        <v>0.37141506174186617</v>
+      </c>
+      <c r="L77" s="2">
+        <f>(E77-E60)/E77</f>
+        <v>0.30987925625776092</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12">
+      <c r="A78" t="s">
+        <v>8</v>
+      </c>
+      <c r="B78">
+        <v>2548.1999999999998</v>
+      </c>
+      <c r="C78">
+        <v>5227.67</v>
+      </c>
+      <c r="D78">
+        <v>14976.9</v>
+      </c>
+      <c r="E78">
+        <v>51918.8</v>
+      </c>
+      <c r="H78" t="s">
+        <v>8</v>
+      </c>
+      <c r="I78" s="2">
+        <f>(B78-B61)/B78</f>
+        <v>-3.3015461894670792E-2</v>
+      </c>
+      <c r="J78" s="2">
+        <f>(C78-C61)/C78</f>
+        <v>0.43197638718587822</v>
+      </c>
+      <c r="K78" s="2">
+        <f>(D78-D61)/D78</f>
+        <v>0.39895505745514753</v>
+      </c>
+      <c r="L78" s="2">
+        <f>(E78-E61)/E78</f>
+        <v>0.22757844942487124</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12">
+      <c r="A79" t="s">
+        <v>9</v>
+      </c>
+      <c r="B79">
+        <v>3200</v>
+      </c>
+      <c r="C79">
+        <v>7975</v>
+      </c>
+      <c r="D79">
+        <v>27331.3</v>
+      </c>
+      <c r="E79">
+        <v>105044</v>
+      </c>
+      <c r="H79" t="s">
+        <v>9</v>
+      </c>
+      <c r="I79" s="2">
+        <f>(B79-B62)/B79</f>
+        <v>0.25</v>
+      </c>
+      <c r="J79" s="2">
+        <f>(C79-C62)/C79</f>
+        <v>0.31661442006269591</v>
+      </c>
+      <c r="K79" s="2">
+        <f>(D79-D62)/D79</f>
+        <v>0.36565403036079513</v>
+      </c>
+      <c r="L79" s="2">
+        <f>(E79-E62)/E79</f>
+        <v>0.33716728228171045</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12">
+      <c r="A80" t="s">
+        <v>10</v>
+      </c>
+      <c r="B80">
+        <v>7400</v>
+      </c>
+      <c r="C80">
+        <v>16350</v>
+      </c>
+      <c r="D80">
+        <v>53318.8</v>
+      </c>
+      <c r="E80">
+        <v>198478</v>
+      </c>
+      <c r="H80" t="s">
+        <v>10</v>
+      </c>
+      <c r="I80" s="2">
+        <f>(B80-B63)/B80</f>
+        <v>0.13513513513513514</v>
+      </c>
+      <c r="J80" s="2">
+        <f>(C80-C63)/C80</f>
+        <v>0.25840978593272174</v>
+      </c>
+      <c r="K80" s="2">
+        <f>(D80-D63)/D80</f>
+        <v>0.29140753355289317</v>
+      </c>
+      <c r="L80" s="2">
+        <f>(E80-E63)/E80</f>
+        <v>0.2449893690988422</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12">
+      <c r="A81" t="s">
+        <v>11</v>
+      </c>
+      <c r="B81">
+        <v>9200</v>
+      </c>
+      <c r="C81">
+        <v>21375</v>
+      </c>
+      <c r="D81">
+        <v>71643.8</v>
+      </c>
+      <c r="E81">
+        <v>253588</v>
+      </c>
+      <c r="H81" t="s">
+        <v>11</v>
+      </c>
+      <c r="I81" s="2">
+        <f>(B81-B64)/B81</f>
+        <v>0.18478260869565216</v>
+      </c>
+      <c r="J81" s="2">
+        <f>(C81-C64)/C81</f>
+        <v>0.31228070175438599</v>
+      </c>
+      <c r="K81" s="2">
+        <f>(D81-D64)/D81</f>
+        <v>0.36090073390858668</v>
+      </c>
+      <c r="L81" s="2">
+        <f>(E81-E64)/E81</f>
+        <v>0.29150432985787972</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12">
+      <c r="A82" t="s">
+        <v>12</v>
+      </c>
+      <c r="B82">
+        <v>37800</v>
+      </c>
+      <c r="C82">
+        <v>58775</v>
+      </c>
+      <c r="D82">
+        <v>116231</v>
+      </c>
+      <c r="E82">
+        <v>415041</v>
+      </c>
+      <c r="H82" t="s">
+        <v>12</v>
+      </c>
+      <c r="I82" s="2">
+        <f>(B82-B65)/B82</f>
+        <v>0.65873015873015872</v>
+      </c>
+      <c r="J82" s="2">
+        <f>(C82-C65)/C82</f>
+        <v>0.61037856231390897</v>
+      </c>
+      <c r="K82" s="2">
+        <f>(D82-D65)/D82</f>
+        <v>0.44555411206992968</v>
+      </c>
+      <c r="L82" s="2">
+        <f>(E82-E65)/E82</f>
+        <v>0.40769466149127437</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12">
+      <c r="A83" t="s">
+        <v>13</v>
+      </c>
+      <c r="B83">
+        <v>75900</v>
+      </c>
+      <c r="C83">
+        <v>105950</v>
+      </c>
+      <c r="D83">
+        <v>184725</v>
+      </c>
+      <c r="E83">
+        <v>748452</v>
+      </c>
+      <c r="H83" t="s">
+        <v>13</v>
+      </c>
+      <c r="I83" s="2">
+        <f>(B83-B66)/B83</f>
+        <v>0.45849802371541504</v>
+      </c>
+      <c r="J83" s="2">
+        <f>(C83-C66)/C83</f>
+        <v>0.45894289759320434</v>
+      </c>
+      <c r="K83" s="2">
+        <f>(D83-D66)/D83</f>
+        <v>0.3979916091487346</v>
+      </c>
+      <c r="L83" s="2">
+        <f>(E83-E66)/E83</f>
+        <v>0.5605596618086397</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Did a bit of tuning of null_multiplexer, added results for Linux.
</commit_message>
<xml_diff>
--- a/programs/benchmark-async/results.xlsx
+++ b/programs/benchmark-async/results.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="90" windowWidth="29625" windowHeight="14295"/>
+    <workbookView xWindow="-105" yWindow="90" windowWidth="29625" windowHeight="14295" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="MSVC Win10" sheetId="1" r:id="rId1"/>
+    <sheet name="GCC 7 Linux" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="29">
   <si>
     <t>LLFIO pipe_handle, no locking</t>
   </si>
@@ -76,6 +76,33 @@
   </si>
   <si>
     <t>locking over no locking</t>
+  </si>
+  <si>
+    <t>Total Mins</t>
+  </si>
+  <si>
+    <t>Total Maxs</t>
+  </si>
+  <si>
+    <t>Total Means</t>
+  </si>
+  <si>
+    <t>Total Stddevs</t>
+  </si>
+  <si>
+    <t>Total 50%s</t>
+  </si>
+  <si>
+    <t>Total 95%s</t>
+  </si>
+  <si>
+    <t>Total 99%s</t>
+  </si>
+  <si>
+    <t>Total 99.9%s</t>
+  </si>
+  <si>
+    <t>Total 99.99%s</t>
   </si>
 </sst>
 </file>
@@ -169,7 +196,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$H$77</c:f>
+              <c:f>'MSVC Win10'!$H$77</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -183,7 +210,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$54:$E$54</c:f>
+              <c:f>'MSVC Win10'!$B$54:$E$54</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -204,21 +231,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$I$77:$L$77</c:f>
+              <c:f>'MSVC Win10'!$I$77:$L$77</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.14109586550623454</c:v>
+                  <c:v>0.29294142269463147</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.34469735216933217</c:v>
+                  <c:v>0.34422169522161467</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.37141506174186617</c:v>
+                  <c:v>0.38089782877799944</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.30987925625776092</c:v>
+                  <c:v>0.20483481185177366</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -229,7 +256,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$H$78</c:f>
+              <c:f>'MSVC Win10'!$H$78</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -243,7 +270,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$54:$E$54</c:f>
+              <c:f>'MSVC Win10'!$B$54:$E$54</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -264,21 +291,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$I$78:$L$78</c:f>
+              <c:f>'MSVC Win10'!$I$78:$L$78</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>-3.3015461894670792E-2</c:v>
+                  <c:v>0.22339397842537434</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.43197638718587822</c:v>
+                  <c:v>0.39574511274379892</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.39895505745514753</c:v>
+                  <c:v>0.19276207415791655</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.22757844942487124</c:v>
+                  <c:v>0.22956215167879104</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -289,7 +316,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$H$79</c:f>
+              <c:f>'MSVC Win10'!$H$79</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -303,7 +330,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$54:$E$54</c:f>
+              <c:f>'MSVC Win10'!$B$54:$E$54</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -324,21 +351,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$I$79:$L$79</c:f>
+              <c:f>'MSVC Win10'!$I$79:$L$79</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.25</c:v>
+                  <c:v>0.27272727272727271</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.31661442006269591</c:v>
+                  <c:v>0.30681818181818182</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.36565403036079513</c:v>
+                  <c:v>0.323943661971831</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.33716728228171045</c:v>
+                  <c:v>0.25481421081075956</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -349,7 +376,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$H$80</c:f>
+              <c:f>'MSVC Win10'!$H$80</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -363,7 +390,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$54:$E$54</c:f>
+              <c:f>'MSVC Win10'!$B$54:$E$54</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -384,32 +411,32 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$I$80:$L$80</c:f>
+              <c:f>'MSVC Win10'!$I$80:$L$80</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.13513513513513514</c:v>
+                  <c:v>0.25862068965517243</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.25840978593272174</c:v>
+                  <c:v>0.26940639269406391</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.29140753355289317</c:v>
+                  <c:v>0.244874715261959</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.2449893690988422</c:v>
+                  <c:v>0.18566764527722016</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="154088576"/>
-        <c:axId val="154090880"/>
+        <c:axId val="157037696"/>
+        <c:axId val="157040000"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="154088576"/>
+        <c:axId val="157037696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -439,14 +466,14 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="154090880"/>
+        <c:crossAx val="157040000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="154090880"/>
+        <c:axId val="157040000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -478,7 +505,7 @@
         </c:title>
         <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="154088576"/>
+        <c:crossAx val="157037696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -491,7 +518,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -533,7 +560,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$H$26</c:f>
+              <c:f>'MSVC Win10'!$H$26</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -547,7 +574,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$54:$E$54</c:f>
+              <c:f>'MSVC Win10'!$B$54:$E$54</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -568,21 +595,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$I$26:$L$26</c:f>
+              <c:f>'MSVC Win10'!$I$26:$L$26</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.29754874498314704</c:v>
+                  <c:v>0.3876265443995861</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.17981585220821283</c:v>
+                  <c:v>0.2897921870808936</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.22963049901258883</c:v>
+                  <c:v>0.25614552095547416</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.24316471991590982</c:v>
+                  <c:v>0.27752892203182056</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -593,7 +620,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$H$27</c:f>
+              <c:f>'MSVC Win10'!$H$27</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -607,7 +634,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$54:$E$54</c:f>
+              <c:f>'MSVC Win10'!$B$54:$E$54</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -628,21 +655,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$I$27:$L$27</c:f>
+              <c:f>'MSVC Win10'!$I$27:$L$27</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>-5.7982551054293133E-2</c:v>
+                  <c:v>-0.58891619898946002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-172.1621603376868</c:v>
+                  <c:v>-0.17846466635957875</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.4294342031561524E-2</c:v>
+                  <c:v>-5.7774310292474748E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.3574085988419247E-2</c:v>
+                  <c:v>0.9130498525849986</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -653,7 +680,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$H$28</c:f>
+              <c:f>'MSVC Win10'!$H$28</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -667,7 +694,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$54:$E$54</c:f>
+              <c:f>'MSVC Win10'!$B$54:$E$54</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -688,7 +715,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$I$28:$L$28</c:f>
+              <c:f>'MSVC Win10'!$I$28:$L$28</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="4"/>
@@ -702,7 +729,7 @@
                   <c:v>0.2638888888888889</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.25187533462138317</c:v>
+                  <c:v>0.26535636018989867</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -713,7 +740,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$H$29</c:f>
+              <c:f>'MSVC Win10'!$H$29</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -727,7 +754,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$54:$E$54</c:f>
+              <c:f>'MSVC Win10'!$B$54:$E$54</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -748,7 +775,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$I$29:$L$29</c:f>
+              <c:f>'MSVC Win10'!$I$29:$L$29</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="4"/>
@@ -756,24 +783,24 @@
                   <c:v>0.33333333333333331</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.13793103448275862</c:v>
+                  <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.21967963386727687</c:v>
+                  <c:v>0.25240384615384615</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.22354530127888667</c:v>
+                  <c:v>0.29060484339914661</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="169813504"/>
-        <c:axId val="169815424"/>
+        <c:axId val="157083520"/>
+        <c:axId val="157163520"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="169813504"/>
+        <c:axId val="157083520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -803,14 +830,14 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="169815424"/>
+        <c:crossAx val="157163520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="169815424"/>
+        <c:axId val="157163520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -842,7 +869,7 @@
         </c:title>
         <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="169813504"/>
+        <c:crossAx val="157083520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -855,7 +882,371 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>I/O</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> latencies null multiplexer</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'GCC 7 Linux'!$H$26</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Means</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'MSVC Win10'!$B$54:$E$54</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>64</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'GCC 7 Linux'!$I$26:$L$26</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.39012927345615056</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.28318748895118323</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.27113007000433659</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.2530394320143598</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'GCC 7 Linux'!$H$27</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Stddevs</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'MSVC Win10'!$B$54:$E$54</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>64</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'GCC 7 Linux'!$I$27:$L$27</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.34658693466682716</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.29724289465336468</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.14402909819690124</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.6332930675478197E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'GCC 7 Linux'!$H$28</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>50%s</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'MSVC Win10'!$B$54:$E$54</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>64</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'GCC 7 Linux'!$I$28:$L$28</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.33333333333333331</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.28146721845422851</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.26016750418760465</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'GCC 7 Linux'!$H$29</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>95%s</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'MSVC Win10'!$B$54:$E$54</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>64</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'GCC 7 Linux'!$I$29:$L$29</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1875</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.25701820331424974</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.2151107674288433</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="176940928"/>
+        <c:axId val="145821696"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="176940928"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Handles</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> in i/o multiplexer doing i/o</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="145821696"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="145821696"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Percentage</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> no locking is faster than locking</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="176940928"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -918,6 +1309,41 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1213,8 +1639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="C60" sqref="C60"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A69" sqref="A69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1311,7 +1737,7 @@
         <v>1200</v>
       </c>
       <c r="E7">
-        <v>4700</v>
+        <v>4600</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1319,16 +1745,16 @@
         <v>6</v>
       </c>
       <c r="B8" s="1">
-        <v>349408000</v>
-      </c>
-      <c r="C8" s="1">
-        <v>447648000</v>
+        <v>1472000</v>
+      </c>
+      <c r="C8">
+        <v>686900</v>
       </c>
       <c r="D8">
-        <v>387200</v>
+        <v>973700</v>
       </c>
       <c r="E8">
-        <v>379100</v>
+        <v>522400</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1336,16 +1762,16 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>152.97</v>
+        <v>120.738</v>
       </c>
       <c r="C9">
-        <v>457.24200000000002</v>
+        <v>389.22300000000001</v>
       </c>
       <c r="D9">
-        <v>1509.67</v>
+        <v>1433.72</v>
       </c>
       <c r="E9">
-        <v>5767.38</v>
+        <v>5657.96</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1353,16 +1779,16 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>66587.199999999997</v>
+        <v>266.98399999999998</v>
       </c>
       <c r="C10">
-        <v>87215.2</v>
+        <v>370.96300000000002</v>
       </c>
       <c r="D10">
-        <v>944.99699999999996</v>
+        <v>728.06500000000005</v>
       </c>
       <c r="E10">
-        <v>3311.88</v>
+        <v>1619.09</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1379,7 +1805,7 @@
         <v>1325</v>
       </c>
       <c r="E11">
-        <v>5142.1899999999996</v>
+        <v>5139.0600000000004</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -1390,13 +1816,13 @@
         <v>200</v>
       </c>
       <c r="C12">
-        <v>625</v>
+        <v>525</v>
       </c>
       <c r="D12">
-        <v>2131.25</v>
+        <v>1943.75</v>
       </c>
       <c r="E12">
-        <v>8335.94</v>
+        <v>7929.69</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -1404,16 +1830,16 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="C13">
-        <v>950</v>
+        <v>725</v>
       </c>
       <c r="D13">
-        <v>3287.5</v>
+        <v>2631.25</v>
       </c>
       <c r="E13">
-        <v>12454.7</v>
+        <v>10550</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -1421,16 +1847,16 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>1500</v>
+        <v>400</v>
       </c>
       <c r="C14">
-        <v>3800</v>
+        <v>1200</v>
       </c>
       <c r="D14">
-        <v>11725</v>
+        <v>4793.75</v>
       </c>
       <c r="E14">
-        <v>45756.3</v>
+        <v>17779.7</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -1438,16 +1864,16 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>3800</v>
+        <v>2500</v>
       </c>
       <c r="C15">
-        <v>9250</v>
+        <v>6475</v>
       </c>
       <c r="D15">
-        <v>27293.8</v>
+        <v>22375</v>
       </c>
       <c r="E15">
-        <v>79676.600000000006</v>
+        <v>48004.7</v>
       </c>
     </row>
     <row r="18" spans="1:12">
@@ -1510,19 +1936,19 @@
         <v>2</v>
       </c>
       <c r="I21" s="2">
-        <f>(B21-B4)/B21</f>
+        <f t="shared" ref="I21:I32" si="0">(B21-B4)/B21</f>
         <v>0.54545454545454541</v>
       </c>
       <c r="J21" s="2">
-        <f>(C21-C4)/C21</f>
+        <f t="shared" ref="J21:J32" si="1">(C21-C4)/C21</f>
         <v>0.19424460431654683</v>
       </c>
       <c r="K21" s="2">
-        <f>(D21-D4)/D21</f>
+        <f t="shared" ref="K21:K32" si="2">(D21-D4)/D21</f>
         <v>6.5517241379310295E-2</v>
       </c>
       <c r="L21" s="2">
-        <f>(E21-E4)/E21</f>
+        <f t="shared" ref="L21:L32" si="3">(E21-E4)/E21</f>
         <v>2.1922807017542715E-3</v>
       </c>
     </row>
@@ -1546,19 +1972,19 @@
         <v>3</v>
       </c>
       <c r="I22" s="2">
-        <f>(B22-B5)/B22</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="J22" s="2">
-        <f>(C22-C5)/C22</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K22" s="2" t="e">
-        <f>(D22-D5)/D22</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L22" s="2">
-        <f>(E22-E5)/E22</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -1582,19 +2008,19 @@
         <v>4</v>
       </c>
       <c r="I23" s="2">
-        <f>(B23-B6)/B23</f>
+        <f t="shared" si="0"/>
         <v>-0.42857142857142877</v>
       </c>
       <c r="J23" s="2">
-        <f>(C23-C6)/C23</f>
+        <f t="shared" si="1"/>
         <v>0.17391304347826086</v>
       </c>
       <c r="K23" s="2">
-        <f>(D23-D6)/D23</f>
+        <f t="shared" si="2"/>
         <v>-1.651162790697674</v>
       </c>
       <c r="L23" s="2">
-        <f>(E23-E6)/E23</f>
+        <f t="shared" si="3"/>
         <v>-0.29670785655510001</v>
       </c>
     </row>
@@ -1612,62 +2038,62 @@
         <v>1600</v>
       </c>
       <c r="E24">
-        <v>6400</v>
+        <v>6500</v>
       </c>
       <c r="H24" t="s">
         <v>5</v>
       </c>
       <c r="I24" s="2">
-        <f>(B24-B7)/B24</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J24" s="2">
-        <f>(C24-C7)/C24</f>
+        <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
       <c r="K24" s="2">
-        <f>(D24-D7)/D24</f>
+        <f t="shared" si="2"/>
         <v>0.25</v>
       </c>
       <c r="L24" s="2">
-        <f>(E24-E7)/E24</f>
-        <v>0.265625</v>
+        <f t="shared" si="3"/>
+        <v>0.29230769230769232</v>
       </c>
     </row>
     <row r="25" spans="1:12">
       <c r="A25" t="s">
         <v>6</v>
       </c>
-      <c r="B25" s="1">
-        <v>266671000</v>
-      </c>
-      <c r="C25" s="1">
-        <v>1736700</v>
+      <c r="B25">
+        <v>278700</v>
+      </c>
+      <c r="C25">
+        <v>357600</v>
       </c>
       <c r="D25">
-        <v>258800</v>
-      </c>
-      <c r="E25">
-        <v>680900</v>
+        <v>652100</v>
+      </c>
+      <c r="E25" s="1">
+        <v>12325800</v>
       </c>
       <c r="H25" t="s">
         <v>6</v>
       </c>
       <c r="I25" s="2">
-        <f>(B25-B8)/B25</f>
-        <v>-0.31025870829599017</v>
+        <f t="shared" si="0"/>
+        <v>-4.2816648726228923</v>
       </c>
       <c r="J25" s="2">
-        <f>(C25-C8)/C25</f>
-        <v>-256.75781654862669</v>
+        <f t="shared" si="1"/>
+        <v>-0.92086129753914991</v>
       </c>
       <c r="K25" s="2">
-        <f>(D25-D8)/D25</f>
-        <v>-0.49613601236476046</v>
+        <f t="shared" si="2"/>
+        <v>-0.49317589326790368</v>
       </c>
       <c r="L25" s="2">
-        <f>(E25-E8)/E25</f>
-        <v>0.44323689234836244</v>
+        <f t="shared" si="3"/>
+        <v>0.95761735546577098</v>
       </c>
     </row>
     <row r="26" spans="1:12">
@@ -1675,35 +2101,35 @@
         <v>7</v>
       </c>
       <c r="B26">
-        <v>217.76599999999999</v>
+        <v>197.16399999999999</v>
       </c>
       <c r="C26">
-        <v>557.48699999999997</v>
+        <v>548.04100000000005</v>
       </c>
       <c r="D26">
-        <v>1959.67</v>
+        <v>1927.42</v>
       </c>
       <c r="E26">
-        <v>7620.39</v>
+        <v>7831.4</v>
       </c>
       <c r="H26" t="s">
         <v>7</v>
       </c>
       <c r="I26" s="2">
-        <f>(B26-B9)/B26</f>
-        <v>0.29754874498314704</v>
+        <f t="shared" si="0"/>
+        <v>0.3876265443995861</v>
       </c>
       <c r="J26" s="2">
-        <f>(C26-C9)/C26</f>
-        <v>0.17981585220821283</v>
+        <f t="shared" si="1"/>
+        <v>0.2897921870808936</v>
       </c>
       <c r="K26" s="2">
-        <f>(D26-D9)/D26</f>
-        <v>0.22963049901258883</v>
+        <f t="shared" si="2"/>
+        <v>0.25614552095547416</v>
       </c>
       <c r="L26" s="2">
-        <f>(E26-E9)/E26</f>
-        <v>0.24316471991590982</v>
+        <f t="shared" si="3"/>
+        <v>0.27752892203182056</v>
       </c>
     </row>
     <row r="27" spans="1:12">
@@ -1711,35 +2137,35 @@
         <v>8</v>
       </c>
       <c r="B27">
-        <v>62937.9</v>
+        <v>168.029</v>
       </c>
       <c r="C27">
-        <v>503.66199999999998</v>
+        <v>314.78500000000003</v>
       </c>
       <c r="D27">
-        <v>958.70100000000002</v>
+        <v>688.29899999999998</v>
       </c>
       <c r="E27">
-        <v>3574.9</v>
+        <v>18620.900000000001</v>
       </c>
       <c r="H27" t="s">
         <v>8</v>
       </c>
       <c r="I27" s="2">
-        <f>(B27-B10)/B27</f>
-        <v>-5.7982551054293133E-2</v>
+        <f t="shared" si="0"/>
+        <v>-0.58891619898946002</v>
       </c>
       <c r="J27" s="2">
-        <f>(C27-C10)/C27</f>
-        <v>-172.1621603376868</v>
+        <f t="shared" si="1"/>
+        <v>-0.17846466635957875</v>
       </c>
       <c r="K27" s="2">
-        <f>(D27-D10)/D27</f>
-        <v>1.4294342031561524E-2</v>
+        <f t="shared" si="2"/>
+        <v>-5.7774310292474748E-2</v>
       </c>
       <c r="L27" s="2">
-        <f>(E27-E10)/E27</f>
-        <v>7.3574085988419247E-2</v>
+        <f t="shared" si="3"/>
+        <v>0.9130498525849986</v>
       </c>
     </row>
     <row r="28" spans="1:12">
@@ -1756,26 +2182,26 @@
         <v>1800</v>
       </c>
       <c r="E28">
-        <v>6873.44</v>
+        <v>6995.31</v>
       </c>
       <c r="H28" t="s">
         <v>9</v>
       </c>
       <c r="I28" s="2">
-        <f>(B28-B11)/B28</f>
+        <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
       <c r="J28" s="2">
-        <f>(C28-C11)/C28</f>
+        <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
       <c r="K28" s="2">
-        <f>(D28-D11)/D28</f>
+        <f t="shared" si="2"/>
         <v>0.2638888888888889</v>
       </c>
       <c r="L28" s="2">
-        <f>(E28-E11)/E28</f>
-        <v>0.25187533462138317</v>
+        <f t="shared" si="3"/>
+        <v>0.26535636018989867</v>
       </c>
     </row>
     <row r="29" spans="1:12">
@@ -1786,32 +2212,32 @@
         <v>300</v>
       </c>
       <c r="C29">
-        <v>725</v>
+        <v>700</v>
       </c>
       <c r="D29">
-        <v>2731.25</v>
+        <v>2600</v>
       </c>
       <c r="E29">
-        <v>10735.9</v>
+        <v>11178.1</v>
       </c>
       <c r="H29" t="s">
         <v>10</v>
       </c>
       <c r="I29" s="2">
-        <f>(B29-B12)/B29</f>
+        <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="J29" s="2">
-        <f>(C29-C12)/C29</f>
-        <v>0.13793103448275862</v>
+        <f t="shared" si="1"/>
+        <v>0.25</v>
       </c>
       <c r="K29" s="2">
-        <f>(D29-D12)/D29</f>
-        <v>0.21967963386727687</v>
+        <f t="shared" si="2"/>
+        <v>0.25240384615384615</v>
       </c>
       <c r="L29" s="2">
-        <f>(E29-E12)/E29</f>
-        <v>0.22354530127888667</v>
+        <f t="shared" si="3"/>
+        <v>0.29060484339914661</v>
       </c>
     </row>
     <row r="30" spans="1:12">
@@ -1819,35 +2245,35 @@
         <v>11</v>
       </c>
       <c r="B30">
-        <v>400</v>
+        <v>300</v>
       </c>
       <c r="C30">
-        <v>1100</v>
+        <v>1000</v>
       </c>
       <c r="D30">
-        <v>4150</v>
+        <v>3575</v>
       </c>
       <c r="E30">
-        <v>16279.7</v>
+        <v>13909.4</v>
       </c>
       <c r="H30" t="s">
         <v>11</v>
       </c>
       <c r="I30" s="2">
-        <f>(B30-B13)/B30</f>
-        <v>0.25</v>
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
       </c>
       <c r="J30" s="2">
-        <f>(C30-C13)/C30</f>
-        <v>0.13636363636363635</v>
+        <f t="shared" si="1"/>
+        <v>0.27500000000000002</v>
       </c>
       <c r="K30" s="2">
-        <f>(D30-D13)/D30</f>
-        <v>0.20783132530120482</v>
+        <f t="shared" si="2"/>
+        <v>0.26398601398601401</v>
       </c>
       <c r="L30" s="2">
-        <f>(E30-E13)/E30</f>
-        <v>0.23495518959194578</v>
+        <f t="shared" si="3"/>
+        <v>0.24152012308223214</v>
       </c>
     </row>
     <row r="31" spans="1:12">
@@ -1855,35 +2281,35 @@
         <v>12</v>
       </c>
       <c r="B31">
-        <v>1600</v>
+        <v>600</v>
       </c>
       <c r="C31">
-        <v>3825</v>
+        <v>1800</v>
       </c>
       <c r="D31">
-        <v>12643.8</v>
+        <v>6243.75</v>
       </c>
       <c r="E31">
-        <v>49046.9</v>
+        <v>27435.9</v>
       </c>
       <c r="H31" t="s">
         <v>12</v>
       </c>
       <c r="I31" s="2">
-        <f>(B31-B14)/B31</f>
-        <v>6.25E-2</v>
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
       </c>
       <c r="J31" s="2">
-        <f>(C31-C14)/C31</f>
-        <v>6.5359477124183009E-3</v>
+        <f t="shared" si="1"/>
+        <v>0.33333333333333331</v>
       </c>
       <c r="K31" s="2">
-        <f>(D31-D14)/D31</f>
-        <v>7.2668027017194145E-2</v>
+        <f t="shared" si="2"/>
+        <v>0.23223223223223224</v>
       </c>
       <c r="L31" s="2">
-        <f>(E31-E14)/E31</f>
-        <v>6.7090886478044454E-2</v>
+        <f t="shared" si="3"/>
+        <v>0.35195492037804482</v>
       </c>
     </row>
     <row r="32" spans="1:12">
@@ -1891,35 +2317,35 @@
         <v>13</v>
       </c>
       <c r="B32">
-        <v>4100</v>
+        <v>3200</v>
       </c>
       <c r="C32">
-        <v>9950</v>
+        <v>7850</v>
       </c>
       <c r="D32">
-        <v>28087.5</v>
+        <v>24637.5</v>
       </c>
       <c r="E32">
-        <v>86120.3</v>
+        <v>94923.4</v>
       </c>
       <c r="H32" t="s">
         <v>13</v>
       </c>
       <c r="I32" s="2">
-        <f>(B32-B15)/B32</f>
-        <v>7.3170731707317069E-2</v>
+        <f t="shared" si="0"/>
+        <v>0.21875</v>
       </c>
       <c r="J32" s="2">
-        <f>(C32-C15)/C32</f>
-        <v>7.0351758793969849E-2</v>
+        <f t="shared" si="1"/>
+        <v>0.1751592356687898</v>
       </c>
       <c r="K32" s="2">
-        <f>(D32-D15)/D32</f>
-        <v>2.8258121940364957E-2</v>
+        <f t="shared" si="2"/>
+        <v>9.1831557584982237E-2</v>
       </c>
       <c r="L32" s="2">
-        <f>(E32-E15)/E32</f>
-        <v>7.4822080276078895E-2</v>
+        <f t="shared" si="3"/>
+        <v>0.49427959807592226</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -2000,16 +2426,16 @@
         <v>5</v>
       </c>
       <c r="B41">
-        <v>1800</v>
+        <v>1200</v>
       </c>
       <c r="C41">
-        <v>3500</v>
+        <v>1100</v>
       </c>
       <c r="D41">
-        <v>10100</v>
+        <v>1100</v>
       </c>
       <c r="E41">
-        <v>35200</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -2017,16 +2443,16 @@
         <v>6</v>
       </c>
       <c r="B42" s="1">
-        <v>1735200</v>
+        <v>3083200</v>
       </c>
       <c r="C42">
-        <v>597300</v>
+        <v>215400</v>
       </c>
       <c r="D42">
-        <v>296900</v>
+        <v>255200</v>
       </c>
       <c r="E42">
-        <v>718000</v>
+        <v>180500</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -2034,16 +2460,16 @@
         <v>7</v>
       </c>
       <c r="B43">
-        <v>2797.39</v>
+        <v>1811.31</v>
       </c>
       <c r="C43">
-        <v>6067.99</v>
+        <v>2111.14</v>
       </c>
       <c r="D43">
-        <v>20019.7</v>
+        <v>1943.07</v>
       </c>
       <c r="E43">
-        <v>82234.8</v>
+        <v>1910.91</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -2051,16 +2477,16 @@
         <v>8</v>
       </c>
       <c r="B44">
-        <v>1916.54</v>
+        <v>2528.3000000000002</v>
       </c>
       <c r="C44">
-        <v>2926.52</v>
+        <v>1365.2</v>
       </c>
       <c r="D44">
-        <v>8824.73</v>
+        <v>1406.6</v>
       </c>
       <c r="E44">
-        <v>37723.599999999999</v>
+        <v>1594.1</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -2068,16 +2494,16 @@
         <v>9</v>
       </c>
       <c r="B45">
-        <v>2200</v>
+        <v>1500</v>
       </c>
       <c r="C45">
-        <v>5175</v>
+        <v>1500</v>
       </c>
       <c r="D45">
-        <v>16875</v>
+        <v>1412.5</v>
       </c>
       <c r="E45">
-        <v>67831.3</v>
+        <v>1468.75</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -2085,16 +2511,16 @@
         <v>10</v>
       </c>
       <c r="B46">
-        <v>6000</v>
+        <v>4000</v>
       </c>
       <c r="C46">
-        <v>11650</v>
+        <v>4075</v>
       </c>
       <c r="D46">
-        <v>37200</v>
+        <v>3900</v>
       </c>
       <c r="E46">
-        <v>144358</v>
+        <v>4026.56</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -2102,16 +2528,16 @@
         <v>11</v>
       </c>
       <c r="B47">
-        <v>7000</v>
+        <v>4500</v>
       </c>
       <c r="C47">
-        <v>14150</v>
+        <v>4650</v>
       </c>
       <c r="D47">
-        <v>44187.5</v>
+        <v>4468.75</v>
       </c>
       <c r="E47">
-        <v>175428</v>
+        <v>4673.4399999999996</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -2119,16 +2545,16 @@
         <v>12</v>
       </c>
       <c r="B48">
-        <v>10900</v>
+        <v>7400</v>
       </c>
       <c r="C48">
-        <v>23175</v>
+        <v>9175</v>
       </c>
       <c r="D48">
-        <v>62856.3</v>
+        <v>11468.8</v>
       </c>
       <c r="E48">
-        <v>237444</v>
+        <v>16151.6</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -2136,16 +2562,16 @@
         <v>13</v>
       </c>
       <c r="B49">
-        <v>36300</v>
+        <v>25200</v>
       </c>
       <c r="C49">
-        <v>60025</v>
+        <v>34625</v>
       </c>
       <c r="D49">
-        <v>116219</v>
+        <v>42962.5</v>
       </c>
       <c r="E49">
-        <v>340753</v>
+        <v>54842.2</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -2226,33 +2652,33 @@
         <v>5</v>
       </c>
       <c r="B58">
-        <v>1900</v>
+        <v>1200</v>
       </c>
       <c r="C58">
-        <v>3800</v>
+        <v>1200</v>
       </c>
       <c r="D58">
-        <v>10900</v>
+        <v>1100</v>
       </c>
       <c r="E58">
-        <v>38900</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="59" spans="1:5">
       <c r="A59" t="s">
         <v>6</v>
       </c>
-      <c r="B59" s="1">
-        <v>2051500</v>
+      <c r="B59">
+        <v>513900</v>
       </c>
       <c r="C59">
-        <v>535800</v>
+        <v>157300</v>
       </c>
       <c r="D59">
-        <v>493400</v>
+        <v>341600</v>
       </c>
       <c r="E59" s="1">
-        <v>3511800</v>
+        <v>1012700</v>
       </c>
     </row>
     <row r="60" spans="1:5">
@@ -2260,16 +2686,16 @@
         <v>7</v>
       </c>
       <c r="B60">
-        <v>3307.03</v>
+        <v>2060.8000000000002</v>
       </c>
       <c r="C60">
-        <v>6425</v>
+        <v>1872.07</v>
       </c>
       <c r="D60">
-        <v>20738.400000000001</v>
+        <v>1945.51</v>
       </c>
       <c r="E60">
-        <v>84476.3</v>
+        <v>2109.12</v>
       </c>
     </row>
     <row r="61" spans="1:5">
@@ -2277,16 +2703,16 @@
         <v>8</v>
       </c>
       <c r="B61">
-        <v>2632.33</v>
+        <v>1254.1099999999999</v>
       </c>
       <c r="C61">
-        <v>2969.44</v>
+        <v>1071.6400000000001</v>
       </c>
       <c r="D61">
-        <v>9001.7900000000009</v>
+        <v>1597.54</v>
       </c>
       <c r="E61">
-        <v>40103.199999999997</v>
+        <v>2137.21</v>
       </c>
     </row>
     <row r="62" spans="1:5">
@@ -2294,16 +2720,16 @@
         <v>9</v>
       </c>
       <c r="B62">
-        <v>2400</v>
+        <v>1600</v>
       </c>
       <c r="C62">
-        <v>5450</v>
+        <v>1525</v>
       </c>
       <c r="D62">
-        <v>17337.5</v>
+        <v>1500</v>
       </c>
       <c r="E62">
-        <v>69626.600000000006</v>
+        <v>1571.88</v>
       </c>
     </row>
     <row r="63" spans="1:5">
@@ -2311,16 +2737,16 @@
         <v>10</v>
       </c>
       <c r="B63">
-        <v>6400</v>
+        <v>4300</v>
       </c>
       <c r="C63">
-        <v>12125</v>
+        <v>4000</v>
       </c>
       <c r="D63">
-        <v>37781.300000000003</v>
+        <v>4143.75</v>
       </c>
       <c r="E63">
-        <v>149853</v>
+        <v>4207.8100000000004</v>
       </c>
     </row>
     <row r="64" spans="1:5">
@@ -2328,16 +2754,16 @@
         <v>11</v>
       </c>
       <c r="B64">
-        <v>7500</v>
+        <v>4800</v>
       </c>
       <c r="C64">
-        <v>14700</v>
+        <v>4700</v>
       </c>
       <c r="D64">
-        <v>45787.5</v>
+        <v>4781.25</v>
       </c>
       <c r="E64">
-        <v>179666</v>
+        <v>4868.75</v>
       </c>
     </row>
     <row r="65" spans="1:12">
@@ -2345,16 +2771,16 @@
         <v>12</v>
       </c>
       <c r="B65">
-        <v>12900</v>
+        <v>7700</v>
       </c>
       <c r="C65">
-        <v>22900</v>
+        <v>8900</v>
       </c>
       <c r="D65">
-        <v>64443.8</v>
+        <v>14812.5</v>
       </c>
       <c r="E65">
-        <v>245831</v>
+        <v>19932.8</v>
       </c>
     </row>
     <row r="66" spans="1:12">
@@ -2362,16 +2788,16 @@
         <v>13</v>
       </c>
       <c r="B66">
-        <v>41100</v>
+        <v>25700</v>
       </c>
       <c r="C66">
-        <v>57325</v>
+        <v>28525</v>
       </c>
       <c r="D66">
-        <v>111206</v>
+        <v>43850</v>
       </c>
       <c r="E66">
-        <v>328900</v>
+        <v>64629.7</v>
       </c>
     </row>
     <row r="69" spans="1:12">
@@ -2434,19 +2860,19 @@
         <v>2</v>
       </c>
       <c r="I72" s="2">
-        <f>(B72-B55)/B72</f>
+        <f t="shared" ref="I72:I83" si="4">(B72-B55)/B72</f>
         <v>0.4478908188585608</v>
       </c>
       <c r="J72" s="2">
-        <f>(C72-C55)/C72</f>
+        <f t="shared" ref="J72:J83" si="5">(C72-C55)/C72</f>
         <v>0.24919354838709681</v>
       </c>
       <c r="K72" s="2">
-        <f>(D72-D55)/D72</f>
+        <f t="shared" ref="K72:K83" si="6">(D72-D55)/D72</f>
         <v>0.27489636608344548</v>
       </c>
       <c r="L72" s="2">
-        <f>(E72-E55)/E72</f>
+        <f t="shared" ref="L72:L83" si="7">(E72-E55)/E72</f>
         <v>7.4375545851528418E-2</v>
       </c>
     </row>
@@ -2470,19 +2896,19 @@
         <v>3</v>
       </c>
       <c r="I73" s="2">
-        <f>(B73-B56)/B73</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J73" s="2">
-        <f>(C73-C56)/C73</f>
+        <f t="shared" si="5"/>
         <v>0.99999997893708081</v>
       </c>
       <c r="K73" s="2">
-        <f>(D73-D56)/D73</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="L73" s="2">
-        <f>(E73-E56)/E73</f>
+        <f t="shared" si="7"/>
         <v>0.99999998288766423</v>
       </c>
     </row>
@@ -2506,19 +2932,19 @@
         <v>4</v>
       </c>
       <c r="I74" s="2">
-        <f>(B74-B57)/B74</f>
+        <f t="shared" si="4"/>
         <v>0.99998720302676247</v>
       </c>
       <c r="J74" s="2">
-        <f>(C74-C57)/C74</f>
+        <f t="shared" si="5"/>
         <v>0.99998599051550408</v>
       </c>
       <c r="K74" s="2">
-        <f>(D74-D57)/D74</f>
+        <f t="shared" si="6"/>
         <v>0.99997296168590577</v>
       </c>
       <c r="L74" s="2">
-        <f>(E74-E57)/E74</f>
+        <f t="shared" si="7"/>
         <v>0.9999276132016216</v>
       </c>
     </row>
@@ -2527,71 +2953,71 @@
         <v>5</v>
       </c>
       <c r="B75">
-        <v>2500</v>
+        <v>1600</v>
       </c>
       <c r="C75">
-        <v>4800</v>
+        <v>1600</v>
       </c>
       <c r="D75">
-        <v>13900</v>
+        <v>1500</v>
       </c>
       <c r="E75">
-        <v>51700</v>
+        <v>1600</v>
       </c>
       <c r="H75" t="s">
         <v>5</v>
       </c>
       <c r="I75" s="2">
-        <f>(B75-B58)/B75</f>
-        <v>0.24</v>
+        <f t="shared" si="4"/>
+        <v>0.25</v>
       </c>
       <c r="J75" s="2">
-        <f>(C75-C58)/C75</f>
-        <v>0.20833333333333334</v>
+        <f t="shared" si="5"/>
+        <v>0.25</v>
       </c>
       <c r="K75" s="2">
-        <f>(D75-D58)/D75</f>
-        <v>0.21582733812949639</v>
+        <f t="shared" si="6"/>
+        <v>0.26666666666666666</v>
       </c>
       <c r="L75" s="2">
-        <f>(E75-E58)/E75</f>
-        <v>0.24758220502901354</v>
+        <f t="shared" si="7"/>
+        <v>0.3125</v>
       </c>
     </row>
     <row r="76" spans="1:12">
       <c r="A76" t="s">
         <v>6</v>
       </c>
-      <c r="B76" s="1">
-        <v>1107800</v>
+      <c r="B76">
+        <v>310600</v>
       </c>
       <c r="C76">
-        <v>683700</v>
-      </c>
-      <c r="D76" s="1">
-        <v>1897900</v>
-      </c>
-      <c r="E76" s="1">
-        <v>2647300</v>
+        <v>460000</v>
+      </c>
+      <c r="D76">
+        <v>244500</v>
+      </c>
+      <c r="E76">
+        <v>365700</v>
       </c>
       <c r="H76" t="s">
         <v>6</v>
       </c>
       <c r="I76" s="2">
-        <f>(B76-B59)/B76</f>
-        <v>-0.85186856833363422</v>
+        <f t="shared" si="4"/>
+        <v>-0.65453960077269802</v>
       </c>
       <c r="J76" s="2">
-        <f>(C76-C59)/C76</f>
-        <v>0.21632294866169371</v>
+        <f t="shared" si="5"/>
+        <v>0.65804347826086962</v>
       </c>
       <c r="K76" s="2">
-        <f>(D76-D59)/D76</f>
-        <v>0.74002845250013172</v>
+        <f t="shared" si="6"/>
+        <v>-0.39713701431492843</v>
       </c>
       <c r="L76" s="2">
-        <f>(E76-E59)/E76</f>
-        <v>-0.32655913572318968</v>
+        <f t="shared" si="7"/>
+        <v>-1.7692097347552638</v>
       </c>
     </row>
     <row r="77" spans="1:12">
@@ -2599,35 +3025,35 @@
         <v>7</v>
       </c>
       <c r="B77">
-        <v>3850.29</v>
+        <v>2914.61</v>
       </c>
       <c r="C77">
-        <v>9804.6299999999992</v>
+        <v>2854.73</v>
       </c>
       <c r="D77">
-        <v>32992.199999999997</v>
+        <v>3142.47</v>
       </c>
       <c r="E77">
-        <v>122408</v>
+        <v>2652.43</v>
       </c>
       <c r="H77" t="s">
         <v>7</v>
       </c>
       <c r="I77" s="2">
-        <f>(B77-B60)/B77</f>
-        <v>0.14109586550623454</v>
+        <f t="shared" si="4"/>
+        <v>0.29294142269463147</v>
       </c>
       <c r="J77" s="2">
-        <f>(C77-C60)/C77</f>
-        <v>0.34469735216933217</v>
+        <f t="shared" si="5"/>
+        <v>0.34422169522161467</v>
       </c>
       <c r="K77" s="2">
-        <f>(D77-D60)/D77</f>
-        <v>0.37141506174186617</v>
+        <f t="shared" si="6"/>
+        <v>0.38089782877799944</v>
       </c>
       <c r="L77" s="2">
-        <f>(E77-E60)/E77</f>
-        <v>0.30987925625776092</v>
+        <f t="shared" si="7"/>
+        <v>0.20483481185177366</v>
       </c>
     </row>
     <row r="78" spans="1:12">
@@ -2635,35 +3061,35 @@
         <v>8</v>
       </c>
       <c r="B78">
-        <v>2548.1999999999998</v>
+        <v>1614.86</v>
       </c>
       <c r="C78">
-        <v>5227.67</v>
+        <v>1773.49</v>
       </c>
       <c r="D78">
-        <v>14976.9</v>
+        <v>1979.02</v>
       </c>
       <c r="E78">
-        <v>51918.8</v>
+        <v>2774.02</v>
       </c>
       <c r="H78" t="s">
         <v>8</v>
       </c>
       <c r="I78" s="2">
-        <f>(B78-B61)/B78</f>
-        <v>-3.3015461894670792E-2</v>
+        <f t="shared" si="4"/>
+        <v>0.22339397842537434</v>
       </c>
       <c r="J78" s="2">
-        <f>(C78-C61)/C78</f>
-        <v>0.43197638718587822</v>
+        <f t="shared" si="5"/>
+        <v>0.39574511274379892</v>
       </c>
       <c r="K78" s="2">
-        <f>(D78-D61)/D78</f>
-        <v>0.39895505745514753</v>
+        <f t="shared" si="6"/>
+        <v>0.19276207415791655</v>
       </c>
       <c r="L78" s="2">
-        <f>(E78-E61)/E78</f>
-        <v>0.22757844942487124</v>
+        <f t="shared" si="7"/>
+        <v>0.22956215167879104</v>
       </c>
     </row>
     <row r="79" spans="1:12">
@@ -2671,35 +3097,35 @@
         <v>9</v>
       </c>
       <c r="B79">
-        <v>3200</v>
+        <v>2200</v>
       </c>
       <c r="C79">
-        <v>7975</v>
+        <v>2200</v>
       </c>
       <c r="D79">
-        <v>27331.3</v>
+        <v>2218.75</v>
       </c>
       <c r="E79">
-        <v>105044</v>
+        <v>2109.38</v>
       </c>
       <c r="H79" t="s">
         <v>9</v>
       </c>
       <c r="I79" s="2">
-        <f>(B79-B62)/B79</f>
-        <v>0.25</v>
+        <f t="shared" si="4"/>
+        <v>0.27272727272727271</v>
       </c>
       <c r="J79" s="2">
-        <f>(C79-C62)/C79</f>
-        <v>0.31661442006269591</v>
+        <f t="shared" si="5"/>
+        <v>0.30681818181818182</v>
       </c>
       <c r="K79" s="2">
-        <f>(D79-D62)/D79</f>
-        <v>0.36565403036079513</v>
+        <f t="shared" si="6"/>
+        <v>0.323943661971831</v>
       </c>
       <c r="L79" s="2">
-        <f>(E79-E62)/E79</f>
-        <v>0.33716728228171045</v>
+        <f t="shared" si="7"/>
+        <v>0.25481421081075956</v>
       </c>
     </row>
     <row r="80" spans="1:12">
@@ -2707,35 +3133,35 @@
         <v>10</v>
       </c>
       <c r="B80">
-        <v>7400</v>
+        <v>5800</v>
       </c>
       <c r="C80">
-        <v>16350</v>
+        <v>5475</v>
       </c>
       <c r="D80">
-        <v>53318.8</v>
+        <v>5487.5</v>
       </c>
       <c r="E80">
-        <v>198478</v>
+        <v>5167.1899999999996</v>
       </c>
       <c r="H80" t="s">
         <v>10</v>
       </c>
       <c r="I80" s="2">
-        <f>(B80-B63)/B80</f>
-        <v>0.13513513513513514</v>
+        <f t="shared" si="4"/>
+        <v>0.25862068965517243</v>
       </c>
       <c r="J80" s="2">
-        <f>(C80-C63)/C80</f>
-        <v>0.25840978593272174</v>
+        <f t="shared" si="5"/>
+        <v>0.26940639269406391</v>
       </c>
       <c r="K80" s="2">
-        <f>(D80-D63)/D80</f>
-        <v>0.29140753355289317</v>
+        <f t="shared" si="6"/>
+        <v>0.244874715261959</v>
       </c>
       <c r="L80" s="2">
-        <f>(E80-E63)/E80</f>
-        <v>0.2449893690988422</v>
+        <f t="shared" si="7"/>
+        <v>0.18566764527722016</v>
       </c>
     </row>
     <row r="81" spans="1:12">
@@ -2743,35 +3169,35 @@
         <v>11</v>
       </c>
       <c r="B81">
-        <v>9200</v>
+        <v>6700</v>
       </c>
       <c r="C81">
-        <v>21375</v>
+        <v>6450</v>
       </c>
       <c r="D81">
-        <v>71643.8</v>
+        <v>6893.75</v>
       </c>
       <c r="E81">
-        <v>253588</v>
+        <v>7621.88</v>
       </c>
       <c r="H81" t="s">
         <v>11</v>
       </c>
       <c r="I81" s="2">
-        <f>(B81-B64)/B81</f>
-        <v>0.18478260869565216</v>
+        <f t="shared" si="4"/>
+        <v>0.28358208955223879</v>
       </c>
       <c r="J81" s="2">
-        <f>(C81-C64)/C81</f>
-        <v>0.31228070175438599</v>
+        <f t="shared" si="5"/>
+        <v>0.27131782945736432</v>
       </c>
       <c r="K81" s="2">
-        <f>(D81-D64)/D81</f>
-        <v>0.36090073390858668</v>
+        <f t="shared" si="6"/>
+        <v>0.30643699002719854</v>
       </c>
       <c r="L81" s="2">
-        <f>(E81-E64)/E81</f>
-        <v>0.29150432985787972</v>
+        <f t="shared" si="7"/>
+        <v>0.36121403118390738</v>
       </c>
     </row>
     <row r="82" spans="1:12">
@@ -2779,35 +3205,35 @@
         <v>12</v>
       </c>
       <c r="B82">
-        <v>37800</v>
+        <v>10200</v>
       </c>
       <c r="C82">
-        <v>58775</v>
+        <v>13675</v>
       </c>
       <c r="D82">
-        <v>116231</v>
+        <v>22100</v>
       </c>
       <c r="E82">
-        <v>415041</v>
+        <v>27915.599999999999</v>
       </c>
       <c r="H82" t="s">
         <v>12</v>
       </c>
       <c r="I82" s="2">
-        <f>(B82-B65)/B82</f>
-        <v>0.65873015873015872</v>
+        <f t="shared" si="4"/>
+        <v>0.24509803921568626</v>
       </c>
       <c r="J82" s="2">
-        <f>(C82-C65)/C82</f>
-        <v>0.61037856231390897</v>
+        <f t="shared" si="5"/>
+        <v>0.34917733089579522</v>
       </c>
       <c r="K82" s="2">
-        <f>(D82-D65)/D82</f>
-        <v>0.44555411206992968</v>
+        <f t="shared" si="6"/>
+        <v>0.32975113122171945</v>
       </c>
       <c r="L82" s="2">
-        <f>(E82-E65)/E82</f>
-        <v>0.40769466149127437</v>
+        <f t="shared" si="7"/>
+        <v>0.2859619710842683</v>
       </c>
     </row>
     <row r="83" spans="1:12">
@@ -2815,35 +3241,35 @@
         <v>13</v>
       </c>
       <c r="B83">
-        <v>75900</v>
+        <v>31900</v>
       </c>
       <c r="C83">
-        <v>105950</v>
+        <v>43000</v>
       </c>
       <c r="D83">
-        <v>184725</v>
+        <v>52331.3</v>
       </c>
       <c r="E83">
-        <v>748452</v>
+        <v>91671.9</v>
       </c>
       <c r="H83" t="s">
         <v>13</v>
       </c>
       <c r="I83" s="2">
-        <f>(B83-B66)/B83</f>
-        <v>0.45849802371541504</v>
+        <f t="shared" si="4"/>
+        <v>0.19435736677115986</v>
       </c>
       <c r="J83" s="2">
-        <f>(C83-C66)/C83</f>
-        <v>0.45894289759320434</v>
+        <f t="shared" si="5"/>
+        <v>0.33662790697674416</v>
       </c>
       <c r="K83" s="2">
-        <f>(D83-D66)/D83</f>
-        <v>0.3979916091487346</v>
+        <f t="shared" si="6"/>
+        <v>0.16206935428701374</v>
       </c>
       <c r="L83" s="2">
-        <f>(E83-E66)/E83</f>
-        <v>0.5605596618086397</v>
+        <f t="shared" si="7"/>
+        <v>0.29498897699294985</v>
       </c>
     </row>
   </sheetData>
@@ -2854,13 +3280,941 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:L49"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H43" sqref="H43"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>4</v>
+      </c>
+      <c r="D3">
+        <v>16</v>
+      </c>
+      <c r="E3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1">
+        <v>4.5000000000000001E-6</v>
+      </c>
+      <c r="C4" s="1">
+        <v>2.1500000000000002E-6</v>
+      </c>
+      <c r="D4" s="1">
+        <v>4.1250000000000002E-7</v>
+      </c>
+      <c r="E4" s="1">
+        <v>2.0314100000000001E-7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1.9999999999999999E-7</v>
+      </c>
+      <c r="C5" s="1">
+        <v>7.4999999999999997E-8</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1.8749999999999999E-8</v>
+      </c>
+      <c r="E5" s="1">
+        <v>3.1249999999999999E-9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1">
+        <v>2.5000000000000002E-6</v>
+      </c>
+      <c r="C6" s="1">
+        <v>4.9999999999999998E-7</v>
+      </c>
+      <c r="D6" s="1">
+        <v>3.2500000000000001E-7</v>
+      </c>
+      <c r="E6" s="1">
+        <v>1.1249999999999999E-7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>100</v>
+      </c>
+      <c r="D7">
+        <v>600</v>
+      </c>
+      <c r="E7">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>354609</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1359740</v>
+      </c>
+      <c r="D8">
+        <v>862723</v>
+      </c>
+      <c r="E8" s="1">
+        <v>1015430</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>67.698700000000002</v>
+      </c>
+      <c r="C9">
+        <v>227.06899999999999</v>
+      </c>
+      <c r="D9">
+        <v>823.572</v>
+      </c>
+      <c r="E9">
+        <v>3266.72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>200.83500000000001</v>
+      </c>
+      <c r="C10">
+        <v>423.142</v>
+      </c>
+      <c r="D10">
+        <v>809.78099999999995</v>
+      </c>
+      <c r="E10">
+        <v>2007.68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>100</v>
+      </c>
+      <c r="C11">
+        <v>200</v>
+      </c>
+      <c r="D11">
+        <v>750.06200000000001</v>
+      </c>
+      <c r="E11">
+        <v>2981.34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>100</v>
+      </c>
+      <c r="C12">
+        <v>325</v>
+      </c>
+      <c r="D12">
+        <v>1156.31</v>
+      </c>
+      <c r="E12">
+        <v>4851.7299999999996</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>100</v>
+      </c>
+      <c r="C13">
+        <v>450</v>
+      </c>
+      <c r="D13">
+        <v>1543.88</v>
+      </c>
+      <c r="E13">
+        <v>6573.52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>300</v>
+      </c>
+      <c r="C14">
+        <v>800.25</v>
+      </c>
+      <c r="D14">
+        <v>10319.1</v>
+      </c>
+      <c r="E14">
+        <v>18866.099999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>6400</v>
+      </c>
+      <c r="C15">
+        <v>12575.2</v>
+      </c>
+      <c r="D15">
+        <v>27325.9</v>
+      </c>
+      <c r="E15">
+        <v>53393.599999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="H18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>4</v>
+      </c>
+      <c r="D20">
+        <v>16</v>
+      </c>
+      <c r="E20">
+        <v>64</v>
+      </c>
+      <c r="H20" t="s">
+        <v>1</v>
+      </c>
+      <c r="I20">
+        <v>1</v>
+      </c>
+      <c r="J20">
+        <v>4</v>
+      </c>
+      <c r="K20">
+        <v>16</v>
+      </c>
+      <c r="L20">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B21" s="1">
+        <v>8.1000000000000004E-6</v>
+      </c>
+      <c r="C21" s="1">
+        <v>1.07525E-6</v>
+      </c>
+      <c r="D21" s="1">
+        <v>5.6881199999999997E-7</v>
+      </c>
+      <c r="E21" s="1">
+        <v>2.34391E-7</v>
+      </c>
+      <c r="H21" t="s">
+        <v>2</v>
+      </c>
+      <c r="I21" s="2">
+        <f t="shared" ref="I21:L32" si="0">(B21-B4)/B21</f>
+        <v>0.44444444444444448</v>
+      </c>
+      <c r="J21" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.99953499186235772</v>
+      </c>
+      <c r="K21" s="2">
+        <f t="shared" si="0"/>
+        <v>0.27480432902259438</v>
+      </c>
+      <c r="L21" s="2">
+        <f t="shared" si="0"/>
+        <v>0.13332423173244703</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22" s="1">
+        <v>9.9999999999999995E-8</v>
+      </c>
+      <c r="C22" s="1">
+        <v>4.9999999999999998E-8</v>
+      </c>
+      <c r="D22" s="1">
+        <v>1.8749999999999999E-8</v>
+      </c>
+      <c r="E22" s="1">
+        <v>1.5624999999999999E-9</v>
+      </c>
+      <c r="H22" t="s">
+        <v>3</v>
+      </c>
+      <c r="I22" s="2">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="J22" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.5</v>
+      </c>
+      <c r="K22" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L22" s="2">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="A23" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" s="1">
+        <v>1.5E-6</v>
+      </c>
+      <c r="C23" s="1">
+        <v>4.2500000000000001E-7</v>
+      </c>
+      <c r="D23" s="1">
+        <v>2.875E-7</v>
+      </c>
+      <c r="E23" s="1">
+        <v>1.1249999999999999E-7</v>
+      </c>
+      <c r="H23" t="s">
+        <v>4</v>
+      </c>
+      <c r="I23" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.66666666666666674</v>
+      </c>
+      <c r="J23" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.17647058823529405</v>
+      </c>
+      <c r="K23" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.1304347826086957</v>
+      </c>
+      <c r="L23" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="A24" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>200</v>
+      </c>
+      <c r="D24">
+        <v>900</v>
+      </c>
+      <c r="E24">
+        <v>3800</v>
+      </c>
+      <c r="H24" t="s">
+        <v>5</v>
+      </c>
+      <c r="I24" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J24" s="2">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="K24" s="2">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="L24" s="2">
+        <f t="shared" si="0"/>
+        <v>0.36842105263157893</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="A25" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25">
+        <v>977826</v>
+      </c>
+      <c r="C25" s="1">
+        <v>1626140</v>
+      </c>
+      <c r="D25" s="1">
+        <v>1330440</v>
+      </c>
+      <c r="E25" s="1">
+        <v>1020530</v>
+      </c>
+      <c r="H25" t="s">
+        <v>6</v>
+      </c>
+      <c r="I25" s="2">
+        <f t="shared" si="0"/>
+        <v>0.63734958980432099</v>
+      </c>
+      <c r="J25" s="2">
+        <f t="shared" si="0"/>
+        <v>0.16382353302913649</v>
+      </c>
+      <c r="K25" s="2">
+        <f t="shared" si="0"/>
+        <v>0.3515506148341902</v>
+      </c>
+      <c r="L25" s="2">
+        <f t="shared" si="0"/>
+        <v>4.9974033100447807E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="A26" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26">
+        <v>111.005</v>
+      </c>
+      <c r="C26">
+        <v>316.77600000000001</v>
+      </c>
+      <c r="D26">
+        <v>1129.93</v>
+      </c>
+      <c r="E26">
+        <v>4373.3500000000004</v>
+      </c>
+      <c r="H26" t="s">
+        <v>7</v>
+      </c>
+      <c r="I26" s="2">
+        <f t="shared" si="0"/>
+        <v>0.39012927345615056</v>
+      </c>
+      <c r="J26" s="2">
+        <f t="shared" si="0"/>
+        <v>0.28318748895118323</v>
+      </c>
+      <c r="K26" s="2">
+        <f t="shared" si="0"/>
+        <v>0.27113007000433659</v>
+      </c>
+      <c r="L26" s="2">
+        <f t="shared" si="0"/>
+        <v>0.2530394320143598</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="A27" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27">
+        <v>307.363</v>
+      </c>
+      <c r="C27">
+        <v>602.11699999999996</v>
+      </c>
+      <c r="D27">
+        <v>946.03800000000001</v>
+      </c>
+      <c r="E27">
+        <v>2127.5300000000002</v>
+      </c>
+      <c r="H27" t="s">
+        <v>8</v>
+      </c>
+      <c r="I27" s="2">
+        <f t="shared" si="0"/>
+        <v>0.34658693466682716</v>
+      </c>
+      <c r="J27" s="2">
+        <f t="shared" si="0"/>
+        <v>0.29724289465336468</v>
+      </c>
+      <c r="K27" s="2">
+        <f t="shared" si="0"/>
+        <v>0.14402909819690124</v>
+      </c>
+      <c r="L27" s="2">
+        <f t="shared" si="0"/>
+        <v>5.6332930675478197E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
+      <c r="A28" t="s">
+        <v>9</v>
+      </c>
+      <c r="B28">
+        <v>100</v>
+      </c>
+      <c r="C28">
+        <v>300</v>
+      </c>
+      <c r="D28">
+        <v>1043.8800000000001</v>
+      </c>
+      <c r="E28">
+        <v>4029.75</v>
+      </c>
+      <c r="H28" t="s">
+        <v>9</v>
+      </c>
+      <c r="I28" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J28" s="2">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="K28" s="2">
+        <f t="shared" si="0"/>
+        <v>0.28146721845422851</v>
+      </c>
+      <c r="L28" s="2">
+        <f t="shared" si="0"/>
+        <v>0.26016750418760465</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
+      <c r="A29" t="s">
+        <v>10</v>
+      </c>
+      <c r="B29">
+        <v>200</v>
+      </c>
+      <c r="C29">
+        <v>400</v>
+      </c>
+      <c r="D29">
+        <v>1556.31</v>
+      </c>
+      <c r="E29">
+        <v>6181.42</v>
+      </c>
+      <c r="H29" t="s">
+        <v>10</v>
+      </c>
+      <c r="I29" s="2">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="J29" s="2">
+        <f t="shared" si="0"/>
+        <v>0.1875</v>
+      </c>
+      <c r="K29" s="2">
+        <f t="shared" si="0"/>
+        <v>0.25701820331424974</v>
+      </c>
+      <c r="L29" s="2">
+        <f t="shared" si="0"/>
+        <v>0.2151107674288433</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12">
+      <c r="A30" t="s">
+        <v>11</v>
+      </c>
+      <c r="B30">
+        <v>200</v>
+      </c>
+      <c r="C30">
+        <v>600</v>
+      </c>
+      <c r="D30">
+        <v>2081.31</v>
+      </c>
+      <c r="E30">
+        <v>10033</v>
+      </c>
+      <c r="H30" t="s">
+        <v>11</v>
+      </c>
+      <c r="I30" s="2">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="J30" s="2">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+      <c r="K30" s="2">
+        <f t="shared" si="0"/>
+        <v>0.25821718052572651</v>
+      </c>
+      <c r="L30" s="2">
+        <f t="shared" si="0"/>
+        <v>0.34481012658227844</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12">
+      <c r="A31" t="s">
+        <v>12</v>
+      </c>
+      <c r="B31">
+        <v>400</v>
+      </c>
+      <c r="C31">
+        <v>1100</v>
+      </c>
+      <c r="D31">
+        <v>11894.2</v>
+      </c>
+      <c r="E31">
+        <v>23319.200000000001</v>
+      </c>
+      <c r="H31" t="s">
+        <v>12</v>
+      </c>
+      <c r="I31" s="2">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+      <c r="J31" s="2">
+        <f t="shared" si="0"/>
+        <v>0.27250000000000002</v>
+      </c>
+      <c r="K31" s="2">
+        <f t="shared" si="0"/>
+        <v>0.13242588824805371</v>
+      </c>
+      <c r="L31" s="2">
+        <f t="shared" si="0"/>
+        <v>0.1909628117602663</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12">
+      <c r="A32" t="s">
+        <v>13</v>
+      </c>
+      <c r="B32">
+        <v>10700</v>
+      </c>
+      <c r="C32">
+        <v>14775</v>
+      </c>
+      <c r="D32">
+        <v>32181.9</v>
+      </c>
+      <c r="E32">
+        <v>59809.599999999999</v>
+      </c>
+      <c r="H32" t="s">
+        <v>13</v>
+      </c>
+      <c r="I32" s="2">
+        <f t="shared" si="0"/>
+        <v>0.40186915887850466</v>
+      </c>
+      <c r="J32" s="2">
+        <f t="shared" si="0"/>
+        <v>0.14888663282571907</v>
+      </c>
+      <c r="K32" s="2">
+        <f t="shared" si="0"/>
+        <v>0.15089227174281195</v>
+      </c>
+      <c r="L32" s="2">
+        <f t="shared" si="0"/>
+        <v>0.10727374869586154</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" t="s">
+        <v>1</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37">
+        <v>4</v>
+      </c>
+      <c r="D37">
+        <v>16</v>
+      </c>
+      <c r="E37">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" t="s">
+        <v>2</v>
+      </c>
+      <c r="B38" s="1">
+        <v>3.4301000000000002E-5</v>
+      </c>
+      <c r="C38" s="1">
+        <v>4.4801200000000001E-5</v>
+      </c>
+      <c r="D38" s="1">
+        <v>1.91943E-5</v>
+      </c>
+      <c r="E38" s="1">
+        <v>1.1798699999999999E-5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" t="s">
+        <v>3</v>
+      </c>
+      <c r="B39">
+        <v>0.44860800000000001</v>
+      </c>
+      <c r="C39">
+        <v>0.30421100000000001</v>
+      </c>
+      <c r="D39">
+        <v>0.11172600000000001</v>
+      </c>
+      <c r="E39">
+        <v>2.5740699999999998E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" t="s">
+        <v>4</v>
+      </c>
+      <c r="B40">
+        <v>0.199209</v>
+      </c>
+      <c r="C40">
+        <v>0.18801000000000001</v>
+      </c>
+      <c r="D40">
+        <v>0.10736800000000001</v>
+      </c>
+      <c r="E40">
+        <v>2.0590299999999999E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" t="s">
+        <v>20</v>
+      </c>
+      <c r="B41">
+        <v>1200</v>
+      </c>
+      <c r="C41">
+        <v>1200</v>
+      </c>
+      <c r="D41">
+        <v>1300</v>
+      </c>
+      <c r="E41">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" t="s">
+        <v>21</v>
+      </c>
+      <c r="B42" s="1">
+        <v>1010130</v>
+      </c>
+      <c r="C42">
+        <v>555915</v>
+      </c>
+      <c r="D42" s="1">
+        <v>2160760</v>
+      </c>
+      <c r="E42" s="1">
+        <v>1407140</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" t="s">
+        <v>22</v>
+      </c>
+      <c r="B43">
+        <v>2078.52</v>
+      </c>
+      <c r="C43">
+        <v>3052.21</v>
+      </c>
+      <c r="D43">
+        <v>7630.37</v>
+      </c>
+      <c r="E43">
+        <v>23037</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" t="s">
+        <v>23</v>
+      </c>
+      <c r="B44">
+        <v>1593.43</v>
+      </c>
+      <c r="C44">
+        <v>1898.61</v>
+      </c>
+      <c r="D44">
+        <v>5250.77</v>
+      </c>
+      <c r="E44">
+        <v>15035.4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" t="s">
+        <v>24</v>
+      </c>
+      <c r="B45">
+        <v>1600</v>
+      </c>
+      <c r="C45">
+        <v>2850</v>
+      </c>
+      <c r="D45">
+        <v>7256.38</v>
+      </c>
+      <c r="E45">
+        <v>21644.400000000001</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" t="s">
+        <v>25</v>
+      </c>
+      <c r="B46">
+        <v>3600</v>
+      </c>
+      <c r="C46">
+        <v>4550</v>
+      </c>
+      <c r="D46">
+        <v>11500.2</v>
+      </c>
+      <c r="E46">
+        <v>37263.5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" t="s">
+        <v>26</v>
+      </c>
+      <c r="B47">
+        <v>4500</v>
+      </c>
+      <c r="C47">
+        <v>7125.25</v>
+      </c>
+      <c r="D47">
+        <v>19356.8</v>
+      </c>
+      <c r="E47">
+        <v>51470.1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" t="s">
+        <v>27</v>
+      </c>
+      <c r="B48">
+        <v>17400</v>
+      </c>
+      <c r="C48">
+        <v>21025.200000000001</v>
+      </c>
+      <c r="D48">
+        <v>38957.199999999997</v>
+      </c>
+      <c r="E48">
+        <v>95350.9</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" t="s">
+        <v>28</v>
+      </c>
+      <c r="B49">
+        <v>40901</v>
+      </c>
+      <c r="C49">
+        <v>51452</v>
+      </c>
+      <c r="D49">
+        <v>96196.2</v>
+      </c>
+      <c r="E49">
+        <v>246896</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>